<commit_message>
13. Location update for new assets folder in rooms component scss
Location change because of positioning
</commit_message>
<xml_diff>
--- a/DevTracker.xlsx
+++ b/DevTracker.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
   <si>
     <t>NAME</t>
   </si>
@@ -113,47 +113,12 @@
     <t>Changes</t>
   </si>
   <si>
-    <r>
-      <t>300 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>0 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>56d2d5e17e4c7ef5b9408e639fad07ddb648a8f2</t>
   </si>
   <si>
     <t>#1</t>
   </si>
   <si>
-    <t>1. Added "barbican" and "registry" directory</t>
-  </si>
-  <si>
     <t>C:\Users\Staff2\dev\Pirate-Castle&gt;mkdir registry &amp; mkdir barbican</t>
   </si>
   <si>
@@ -164,38 +129,6 @@
   </si>
   <si>
     <t>1 parent 56d2d5e</t>
-  </si>
-  <si>
-    <r>
-      <t>9 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>17 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <t>#0</t>
@@ -235,42 +168,146 @@
     <t>405 changed files</t>
   </si>
   <si>
-    <t> 2 changed files</t>
-  </si>
-  <si>
-    <t> 5 changed files</t>
-  </si>
-  <si>
-    <t> 1 changed file </t>
+    <t>Add "version": "3.2.4", to registry folder</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>1 parent 5a16089</t>
+  </si>
+  <si>
+    <t>157613ac95fb783a249dd083f17e13a22ce90a40</t>
+  </si>
+  <si>
+    <t>30,857 additions and 4 deletions.</t>
+  </si>
+  <si>
+    <t>We need to add dependencies to package.json from ngx-admin/package.json that is not exists. Also you need to check version of dependency that is already exists. You can pick ngx-admin version if it is upper.</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>1 parent 157613a </t>
+  </si>
+  <si>
+    <t>f808899cd659b6f1b7d643304a93c850ef924724</t>
+  </si>
+  <si>
+    <t>1,724 additions and 204 deletions.</t>
+  </si>
+  <si>
+    <t>300 additions and 0 deletions.</t>
+  </si>
+  <si>
+    <t>9 additions and 17 deletions.</t>
+  </si>
+  <si>
+    <t>32,564 additions and 10 deletions.</t>
+  </si>
+  <si>
+    <t>mkdir src/main/webapp/app/ngx-admin;
+cp -R ../ngx-admin/src/app/* src/main/webapp/app/ngx-admin/</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>515 changed files</t>
+  </si>
+  <si>
+    <t>291 changed files </t>
+  </si>
+  <si>
+    <t>1 parent f808899</t>
+  </si>
+  <si>
+    <t>f3d4bd83b06bd8d5cd95ce38960b6a82fb221a5c</t>
+  </si>
+  <si>
+    <t>41,650 additions and 15 deletions.</t>
+  </si>
+  <si>
+    <t>Updated "app.main.ts" file.</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>1 changed file </t>
+  </si>
+  <si>
+    <t>5 changed files</t>
+  </si>
+  <si>
+    <t>1 parent f3d4bd8</t>
+  </si>
+  <si>
+    <t>39858907d928bca6401f2c6e8a0af5a5ec8e9b66</t>
+  </si>
+  <si>
+    <t>35 additions and 232 deletions.</t>
+  </si>
+  <si>
+    <t>1. Version added to README.md </t>
+  </si>
+  <si>
+    <t>2. Added "barbican" and "registry" directory</t>
+  </si>
+  <si>
+    <t>3. Generated jhipster in "barbican" folder </t>
+  </si>
+  <si>
+    <t>4. Added "registry" files from github</t>
+  </si>
+  <si>
+    <t>5. Dependency merge;</t>
+  </si>
+  <si>
+    <t>6. Copy ngx-admin ui-component files;</t>
+  </si>
+  <si>
+    <t>7. ootstrapModule switched to ngx-admin app-module</t>
+  </si>
+  <si>
+    <t>8. Overwrite index.html from ngx-admin</t>
+  </si>
+  <si>
+    <t>cp ../ngx-admin/src/index.html src/main/webapp/index.html</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>1 parent 3985890</t>
+  </si>
+  <si>
+    <t>69dadbfad32c827cecb95c9b367c3de783686e0a</t>
+  </si>
+  <si>
+    <t>51 additions and 79 deletions.</t>
+  </si>
+  <si>
+    <t>9. Fix "Cannot find name 'tinymce'" error </t>
+  </si>
+  <si>
+    <t>cp ../ngx-admin/src/typings.d.ts src/main/webapp/app/ngx-admin/
+and import it in app-module</t>
   </si>
   <si>
     <r>
-      <t>32,564 additions</t>
+      <t>6 changed files</t>
     </r>
     <r>
       <rPr>
-        <sz val="9"/>
+        <sz val="11"/>
         <color rgb="FF24292E"/>
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
-      <t> and </t>
+      <t> </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>10 deletions.</t>
-    </r>
-  </si>
-  <si>
-    <t>3. Added "registry" files from github</t>
-  </si>
-  <si>
-    <t>Add "version": "3.2.4", to registry folder</t>
   </si>
   <si>
     <r>
@@ -281,11 +318,11 @@
         <family val="2"/>
         <scheme val="major"/>
       </rPr>
-      <t>291 changed files</t>
+      <t>3 changed files</t>
     </r>
     <r>
       <rPr>
-        <sz val="9"/>
+        <sz val="11"/>
         <color rgb="FF24292E"/>
         <rFont val="Segoe UI"/>
         <family val="2"/>
@@ -294,22 +331,102 @@
     </r>
   </si>
   <si>
-    <t>#4</t>
-  </si>
-  <si>
-    <t>1 parent 5a16089</t>
-  </si>
-  <si>
-    <t>157613ac95fb783a249dd083f17e13a22ce90a40</t>
-  </si>
-  <si>
-    <t>30,857 additions and 4 deletions.</t>
-  </si>
-  <si>
-    <t>2. Generated jhipster in "barbican" folder </t>
-  </si>
-  <si>
-    <t>0. Version added to README.md </t>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>2 changed files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>8 changed files </t>
+  </si>
+  <si>
+    <t>2 changed files</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>1 parent 69dadbf</t>
+  </si>
+  <si>
+    <t>5d289bfe0f7312af450d76f10b941b4ebd23f8b9</t>
+  </si>
+  <si>
+    <t>123 additions and 10 deletions.</t>
+  </si>
+  <si>
+    <t>10. Fix Error: Cannot find module 'app/pages/pages.module'.</t>
+  </si>
+  <si>
+    <t>Setting a clean path</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <r>
+      <t>3 changed files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>1 parent 5d289bf</t>
+  </si>
+  <si>
+    <t>2e901a51134984e3cf4a46e4f000f9bf629b9d28</t>
+  </si>
+  <si>
+    <t>68 additions and 32 deletions.</t>
+  </si>
+  <si>
+    <t>11. Copy the assets folder</t>
+  </si>
+  <si>
+    <t>cp -R ../ngx-admin/src/assets ./src/main/webapp/app/ngx-admin/</t>
+  </si>
+  <si>
+    <t>39 changed files</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>1 parent 2e901a5</t>
+  </si>
+  <si>
+    <t>0e436298741ae99a17beacbdfc7ce587d7f03fda</t>
+  </si>
+  <si>
+    <t>268 additions and 19 deletions.</t>
+  </si>
+  <si>
+    <t>12. Configure webpack/webpack.common.js to copy assets folder to targ… </t>
+  </si>
+  <si>
+    <t>…et web folder to be able to served from application</t>
   </si>
 </sst>
 </file>
@@ -319,7 +436,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="9"/>
       <color theme="1" tint="0.499984740745262"/>
@@ -380,12 +497,6 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF24292E"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF444D56"/>
       <name val="Consolas"/>
@@ -398,16 +509,29 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="8"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Century Gothic"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
       <sz val="8"/>
-      <color rgb="FF24292E"/>
-      <name val="Segoe UI"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Segoe UI Light"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -456,7 +580,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -521,19 +645,31 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2713,8 +2849,8 @@
   </sheetPr>
   <dimension ref="A1:M327"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -2799,17 +2935,17 @@
       <c r="F13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="24" t="s">
-        <v>42</v>
+      <c r="H13" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K13" t="s">
         <v>22</v>
@@ -2829,28 +2965,28 @@
         <v>12</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="24" t="s">
-        <v>43</v>
+      <c r="H14" s="28" t="s">
+        <v>62</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>25</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="M14" s="22" t="s">
         <v>27</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="3:13" ht="21" customHeight="1">
@@ -2864,28 +3000,28 @@
         <v>12</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>44</v>
+        <v>67</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>18</v>
       </c>
       <c r="J15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="L15" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="M15" s="22" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="3:13" ht="18" customHeight="1">
@@ -2899,28 +3035,28 @@
         <v>12</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>41</v>
+        <v>68</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>18</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="22" t="s">
-        <v>45</v>
+        <v>36</v>
+      </c>
+      <c r="M16" s="24" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="3:13" ht="18" customHeight="1">
@@ -2928,34 +3064,34 @@
         <v>43141</v>
       </c>
       <c r="D17" s="15">
-        <v>0.69374999999999998</v>
+        <v>0.78402777777777777</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>48</v>
+        <v>69</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="I17" s="14" t="s">
         <v>18</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="L17" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>52</v>
+        <v>42</v>
+      </c>
+      <c r="M17" s="24" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="3:13" ht="18" customHeight="1">
@@ -2963,14 +3099,34 @@
         <v>43141</v>
       </c>
       <c r="D18" s="15">
-        <v>0.69374999999999998</v>
+        <v>0.81597222222222221</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="20"/>
+      <c r="F18" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="I18" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" s="24" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="3:13" ht="18" customHeight="1">
@@ -2978,14 +3134,34 @@
         <v>43141</v>
       </c>
       <c r="D19" s="15">
-        <v>0.69374999999999998</v>
+        <v>0.87083333333333324</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="20"/>
+      <c r="F19" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="I19" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19" s="24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="3:13" ht="18" customHeight="1">
@@ -2993,14 +3169,34 @@
         <v>43141</v>
       </c>
       <c r="D20" s="15">
-        <v>0.69374999999999998</v>
+        <v>0.8881944444444444</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="20"/>
+      <c r="F20" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="I20" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L20" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="3:13" ht="18" customHeight="1">
@@ -3008,14 +3204,34 @@
         <v>43141</v>
       </c>
       <c r="D21" s="15">
-        <v>0.69374999999999998</v>
+        <v>0.92847222222222225</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="20"/>
+      <c r="F21" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>82</v>
+      </c>
       <c r="I21" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M21" s="24" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="3:13" ht="18" customHeight="1">
@@ -3023,14 +3239,34 @@
         <v>43141</v>
       </c>
       <c r="D22" s="15">
-        <v>0.69374999999999998</v>
+        <v>0.94097222222222221</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="20"/>
+      <c r="F22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" t="s">
+        <v>81</v>
+      </c>
       <c r="I22" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="L22" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M22" s="24" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="3:13" ht="18" customHeight="1">
@@ -3038,14 +3274,34 @@
         <v>43141</v>
       </c>
       <c r="D23" s="15">
-        <v>0.69374999999999998</v>
+        <v>0.94444444444444453</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="20"/>
+      <c r="F23" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" t="s">
+        <v>93</v>
+      </c>
       <c r="I23" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="L23" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="M23" s="24" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="3:13" ht="18" customHeight="1">
@@ -3053,14 +3309,34 @@
         <v>43141</v>
       </c>
       <c r="D24" s="15">
-        <v>0.69374999999999998</v>
+        <v>0.95277777777777783</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="20"/>
+      <c r="F24" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="H24" t="s">
+        <v>99</v>
+      </c>
       <c r="I24" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="L24" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="M24" s="24" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="3:13" ht="18" customHeight="1">
@@ -3073,7 +3349,12 @@
       <c r="E25" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="20"/>
+      <c r="F25" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>105</v>
+      </c>
       <c r="I25" s="14" t="s">
         <v>18</v>
       </c>
@@ -4456,19 +4737,19 @@
       <c r="C327" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I41:I55 E14:E55 C13:D55 G36:G55 F18:F55 H18:H55 J18:K55">
+  <conditionalFormatting sqref="I41:I55 E14:E55 C13:D55 G36:G55 H25:H55 J25:K55 F26:F55">
     <cfRule type="expression" dxfId="12" priority="4">
       <formula>#REF!="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="G36:G55 F18:F55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="G36:G55 F26:F55">
       <formula1>Courses</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This employee name isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Personnel Info sheet, it will automatically appear in the list." sqref="E46:E55">
       <formula1>Employees</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="H18:H55 I41:I55 J18:J55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="H25:H55 I41:I55 J25:J55">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4521,13 +4802,35 @@
     <hyperlink ref="F16" r:id="rId46" tooltip="2. Generated jhipster in &quot;barbican&quot; folder_x000a__x000a_Application files will be generated in folder: C:\Users\Staff2\dev\Pirate-Castle\barbican_x000a_? Which *type* of application would you like to create? Microservice gateway_x000a_? What is the base name of your application?" display="https://github.com/Spirovanni/Pirate-Castle/commit/5a16089bca5dbf91aff00987f2817cf484984adb"/>
     <hyperlink ref="F15" r:id="rId47" tooltip="1.  Added &quot;barbican&quot; and &quot;registry&quot; directory_x000a__x000a_C:\Users\Staff2\dev\Pirate-Castle&gt;mkdir registry &amp; mkdir barbican" display="https://github.com/Spirovanni/Pirate-Castle/commit/9ba6b022fbe34293ee459f682bf32e0ddde23494"/>
     <hyperlink ref="F14" r:id="rId48" tooltip="0. Version added to README.md_x000a__x000a_First update from GitKraken" display="https://github.com/Spirovanni/Pirate-Castle/commit/56d2d5e17e4c7ef5b9408e639fad07ddb648a8f2"/>
+    <hyperlink ref="F18" r:id="rId49" tooltip="4. Dependency merge;_x000a__x000a_We need to add dependencies to package.json from ngx-admin/package.json that is not exists. Also you need to check version of dependency that is already exists. You can pick ngx-admin version if it is upper." display="https://github.com/Spirovanni/Pirate-Castle/commit/f808899cd659b6f1b7d643304a93c850ef924724"/>
+    <hyperlink ref="J18" r:id="rId50" tooltip="Merged Pull Request: 4. Dependency merge;" display="https://github.com/Spirovanni/Pirate-Castle/pull/5"/>
+    <hyperlink ref="K18" r:id="rId51" display="https://github.com/Spirovanni/Pirate-Castle/commit/157613ac95fb783a249dd083f17e13a22ce90a40"/>
+    <hyperlink ref="F19" r:id="rId52" tooltip="5. Copy ngx-admin ui-component files;_x000a__x000a_mkdir src/main/webapp/app/ngx-admin;_x000a_cp -R ../ngx-admin/src/app/* src/main/webapp/app/ngx-admin/" display="https://github.com/Spirovanni/Pirate-Castle/commit/f3d4bd83b06bd8d5cd95ce38960b6a82fb221a5c"/>
+    <hyperlink ref="J19" r:id="rId53" tooltip="Merged Pull Request: 5. Copy ngx-admin ui-component files;" display="https://github.com/Spirovanni/Pirate-Castle/pull/6"/>
+    <hyperlink ref="K19" r:id="rId54" display="https://github.com/Spirovanni/Pirate-Castle/commit/f808899cd659b6f1b7d643304a93c850ef924724"/>
+    <hyperlink ref="F20" r:id="rId55" tooltip="6. bootstrapModule switched to ngx-admin app-module_x000a__x000a_Updated &quot;app.main.ts&quot; file." display="https://github.com/Spirovanni/Pirate-Castle/commit/39858907d928bca6401f2c6e8a0af5a5ec8e9b66"/>
+    <hyperlink ref="J20" r:id="rId56" tooltip="Merged Pull Request: 6. bootstrapModule switched to ngx-admin app-module" display="https://github.com/Spirovanni/Pirate-Castle/pull/7"/>
+    <hyperlink ref="K20" r:id="rId57" display="https://github.com/Spirovanni/Pirate-Castle/commit/f3d4bd83b06bd8d5cd95ce38960b6a82fb221a5c"/>
+    <hyperlink ref="F21" r:id="rId58" tooltip="7. Overwrite index.html from ngx-admin_x000a__x000a_cp ../ngx-admin/src/index.html src/main/webapp/index.html" display="https://github.com/Spirovanni/Pirate-Castle/commit/69dadbfad32c827cecb95c9b367c3de783686e0a"/>
+    <hyperlink ref="J21" r:id="rId59" tooltip="Merged Pull Request: 7. Overwrite index.html from ngx-admin" display="https://github.com/Spirovanni/Pirate-Castle/pull/8"/>
+    <hyperlink ref="K21" r:id="rId60" display="https://github.com/Spirovanni/Pirate-Castle/commit/39858907d928bca6401f2c6e8a0af5a5ec8e9b66"/>
+    <hyperlink ref="F22" r:id="rId61" tooltip="9. Fix &quot;Cannot find name 'tinymce'&quot; error_x000a__x000a_cp ../ngx-admin/src/typings.d.ts src/main/webapp/app/ngx-admin/_x000a_and import it in app-module" display="https://github.com/Spirovanni/Pirate-Castle/commit/5d289bfe0f7312af450d76f10b941b4ebd23f8b9"/>
+    <hyperlink ref="J22" r:id="rId62" tooltip="Merged Pull Request: 9. Fix &quot;Cannot find name 'tinymce'&quot; error" display="https://github.com/Spirovanni/Pirate-Castle/pull/9"/>
+    <hyperlink ref="K22" r:id="rId63" display="https://github.com/Spirovanni/Pirate-Castle/commit/69dadbfad32c827cecb95c9b367c3de783686e0a"/>
+    <hyperlink ref="F23" r:id="rId64" tooltip="10. Fix Error: Cannot find module 'app/pages/pages.module'._x000a__x000a_Setting a clean path" display="https://github.com/Spirovanni/Pirate-Castle/commit/2e901a51134984e3cf4a46e4f000f9bf629b9d28"/>
+    <hyperlink ref="J23" r:id="rId65" tooltip="Merged Pull Request: 10. Fix Error: Cannot find module 'app/pages/pages.module'." display="https://github.com/Spirovanni/Pirate-Castle/pull/10"/>
+    <hyperlink ref="K23" r:id="rId66" display="https://github.com/Spirovanni/Pirate-Castle/commit/5d289bfe0f7312af450d76f10b941b4ebd23f8b9"/>
+    <hyperlink ref="F24" r:id="rId67" tooltip="11. Copy the assets folder_x000a__x000a_cp -R ../ngx-admin/src/assets ./src/main/webapp/app/ngx-admin/" display="https://github.com/Spirovanni/Pirate-Castle/commit/0e436298741ae99a17beacbdfc7ce587d7f03fda"/>
+    <hyperlink ref="J24" r:id="rId68" tooltip="Merged Pull Request: 11. Copy the assets folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/11"/>
+    <hyperlink ref="K24" r:id="rId69" display="https://github.com/Spirovanni/Pirate-Castle/commit/2e901a51134984e3cf4a46e4f000f9bf629b9d28"/>
+    <hyperlink ref="F25" r:id="rId70" tooltip="12. Configure webpack/webpack.common.js to copy assets folder to targt we…_x000a__x000a_…b folder to be able to served from application" display="https://github.com/Spirovanni/Pirate-Castle/commit/ef60494acc6a007fa853cd1557175e4ce52e4b30"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId49"/>
-  <drawing r:id="rId50"/>
+  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId71"/>
+  <drawing r:id="rId72"/>
   <tableParts count="1">
-    <tablePart r:id="rId51"/>
+    <tablePart r:id="rId73"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4540,9 +4843,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
   <cols>
@@ -4731,9 +5032,7 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
18. String based lazy router loading fixes.
</commit_message>
<xml_diff>
--- a/DevTracker.xlsx
+++ b/DevTracker.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="140">
   <si>
     <t>NAME</t>
   </si>
@@ -428,6 +428,242 @@
   <si>
     <t>…et web folder to be able to served from application</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>4 changed files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>1 parent 0e43629</t>
+  </si>
+  <si>
+    <t>ef60494acc6a007fa853cd1557175e4ce52e4b30</t>
+  </si>
+  <si>
+    <t>42 additions and 43 deletions.</t>
+  </si>
+  <si>
+    <t>13. Location update for new assets folder in rooms component scss </t>
+  </si>
+  <si>
+    <t>Location change because of positioning</t>
+  </si>
+  <si>
+    <t>4 changed files</t>
+  </si>
+  <si>
+    <t>#13</t>
+  </si>
+  <si>
+    <t>1 parent ef60494</t>
+  </si>
+  <si>
+    <t>d8f32fab62468081b5d66cf40e12068572e4c21f</t>
+  </si>
+  <si>
+    <r>
+      <t>28 additions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>56 deletions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>14. Import ngx-admin theme and styles config in vendor.scss</t>
+  </si>
+  <si>
+    <t>Connecting SCSS files</t>
+  </si>
+  <si>
+    <t>3 changed files</t>
+  </si>
+  <si>
+    <t>#14</t>
+  </si>
+  <si>
+    <t>1 parent d8f32fa</t>
+  </si>
+  <si>
+    <t>b82c1fd4f4ea02cceb9f786aac12ea88ac0eb1c9</t>
+  </si>
+  <si>
+    <r>
+      <t>54 additions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>24 deletions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>15. Clear jhipster bootstrap style configs that can conflict with</t>
+  </si>
+  <si>
+    <t>ngx-admin styles</t>
+  </si>
+  <si>
+    <t>#15</t>
+  </si>
+  <si>
+    <t>1 parent b82c1fd </t>
+  </si>
+  <si>
+    <t>327e5ddc66f329c757c423fef55590b75726dfeb</t>
+  </si>
+  <si>
+    <r>
+      <t>54 additions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>292 deletions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>6 changed files</t>
+  </si>
+  <si>
+    <t>npm install echarts@3.7.2 --save;</t>
+  </si>
+  <si>
+    <t>#16</t>
+  </si>
+  <si>
+    <t>1 parent 70338c0</t>
+  </si>
+  <si>
+    <t>d481422865fb0045eecc23700b50649ffd1be0db</t>
+  </si>
+  <si>
+    <r>
+      <t>87 additions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>36 deletions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>#17</t>
+  </si>
+  <si>
+    <t>16. Echarts dependency install and compnent configs applied.</t>
+  </si>
+  <si>
+    <t>17. tinymce and chart components js bundle configs</t>
+  </si>
 </sst>
 </file>
 
@@ -436,7 +672,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="9"/>
       <color theme="1" tint="0.499984740745262"/>
@@ -528,10 +764,23 @@
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="8"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0366D6"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -580,7 +829,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -660,16 +909,22 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2849,8 +3104,8 @@
   </sheetPr>
   <dimension ref="A1:M327"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D25" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -2867,7 +3122,7 @@
     <col min="10" max="10" width="6.42578125" customWidth="1"/>
     <col min="11" max="11" width="16.140625" customWidth="1"/>
     <col min="12" max="12" width="43.5703125" customWidth="1"/>
-    <col min="13" max="13" width="26.5703125" customWidth="1"/>
+    <col min="13" max="13" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:13" ht="14.25"/>
@@ -2970,7 +3225,7 @@
       <c r="G14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="29" t="s">
         <v>62</v>
       </c>
       <c r="I14" s="14" t="s">
@@ -3005,7 +3260,7 @@
       <c r="G15" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="29" t="s">
         <v>61</v>
       </c>
       <c r="I15" s="14" t="s">
@@ -3040,7 +3295,7 @@
       <c r="G16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="29" t="s">
         <v>38</v>
       </c>
       <c r="I16" s="14" t="s">
@@ -3075,7 +3330,7 @@
       <c r="G17" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="H17" s="29" t="s">
         <v>55</v>
       </c>
       <c r="I17" s="14" t="s">
@@ -3110,7 +3365,7 @@
       <c r="G18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="28" t="s">
+      <c r="H18" s="29" t="s">
         <v>84</v>
       </c>
       <c r="I18" s="14" t="s">
@@ -3142,10 +3397,10 @@
       <c r="F19" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="29" t="s">
         <v>54</v>
       </c>
       <c r="I19" s="14" t="s">
@@ -3180,7 +3435,7 @@
       <c r="G20" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="30" t="s">
         <v>83</v>
       </c>
       <c r="I20" s="14" t="s">
@@ -3247,7 +3502,7 @@
       <c r="F22" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="28" t="s">
         <v>80</v>
       </c>
       <c r="H22" t="s">
@@ -3297,7 +3552,7 @@
       <c r="K23" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="L23" s="30" t="s">
+      <c r="L23" s="31" t="s">
         <v>95</v>
       </c>
       <c r="M23" s="24" t="s">
@@ -3332,7 +3587,7 @@
       <c r="K24" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="L24" s="30" t="s">
+      <c r="L24" s="31" t="s">
         <v>102</v>
       </c>
       <c r="M24" s="24" t="s">
@@ -3352,11 +3607,26 @@
       <c r="F25" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="28" t="s">
         <v>105</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="I25" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="L25" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="M25" s="24" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="3:13" ht="18" customHeight="1">
@@ -3369,9 +3639,29 @@
       <c r="E26" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="20"/>
+      <c r="F26" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="I26" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="L26" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="3:13" ht="18" customHeight="1">
@@ -3384,9 +3674,29 @@
       <c r="E27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="20"/>
+      <c r="F27" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>120</v>
+      </c>
       <c r="I27" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L27" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="3:13" ht="18" customHeight="1">
@@ -3399,9 +3709,29 @@
       <c r="E28" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="20"/>
+      <c r="F28" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="I28" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="L28" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="3:13" ht="18" customHeight="1">
@@ -3414,9 +3744,29 @@
       <c r="E29" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="20"/>
+      <c r="F29" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>131</v>
+      </c>
       <c r="I29" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="L29" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="3:13" ht="18" customHeight="1">
@@ -3429,9 +3779,20 @@
       <c r="E30" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="20"/>
+      <c r="F30" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>120</v>
+      </c>
       <c r="I30" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="3:13" ht="18" customHeight="1">
@@ -4737,19 +5098,19 @@
       <c r="C327" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I41:I55 E14:E55 C13:D55 G36:G55 H25:H55 J25:K55 F26:F55">
+  <conditionalFormatting sqref="I41:I55 E14:E55 C13:D55 G36:G55 F31:F55 H31:H55 K30:K55 J31:J55">
     <cfRule type="expression" dxfId="12" priority="4">
       <formula>#REF!="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="G36:G55 F26:F55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="G36:G55 F31:F55">
       <formula1>Courses</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This employee name isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Personnel Info sheet, it will automatically appear in the list." sqref="E46:E55">
       <formula1>Employees</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="H25:H55 I41:I55 J25:J55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="H31:H55 I41:I55 J31:J55">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4824,13 +5185,29 @@
     <hyperlink ref="J24" r:id="rId68" tooltip="Merged Pull Request: 11. Copy the assets folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/11"/>
     <hyperlink ref="K24" r:id="rId69" display="https://github.com/Spirovanni/Pirate-Castle/commit/2e901a51134984e3cf4a46e4f000f9bf629b9d28"/>
     <hyperlink ref="F25" r:id="rId70" tooltip="12. Configure webpack/webpack.common.js to copy assets folder to targt we…_x000a__x000a_…b folder to be able to served from application" display="https://github.com/Spirovanni/Pirate-Castle/commit/ef60494acc6a007fa853cd1557175e4ce52e4b30"/>
+    <hyperlink ref="J25" r:id="rId71" tooltip="Merged Pull Request: 12. Configure webpack/webpack.common.js to copy assets folder to targ…" display="https://github.com/Spirovanni/Pirate-Castle/pull/12"/>
+    <hyperlink ref="K25" r:id="rId72" display="https://github.com/Spirovanni/Pirate-Castle/commit/0e436298741ae99a17beacbdfc7ce587d7f03fda"/>
+    <hyperlink ref="F26" r:id="rId73" tooltip="13. Location update for new assets folder in rooms component scss_x000a__x000a_Location change because of positioning" display="https://github.com/Spirovanni/Pirate-Castle/commit/d8f32fab62468081b5d66cf40e12068572e4c21f"/>
+    <hyperlink ref="J26" r:id="rId74" tooltip="Merged Pull Request: 13. Location update for new assets folder in rooms component scss" display="https://github.com/Spirovanni/Pirate-Castle/pull/13"/>
+    <hyperlink ref="K26" r:id="rId75" display="https://github.com/Spirovanni/Pirate-Castle/commit/ef60494acc6a007fa853cd1557175e4ce52e4b30"/>
+    <hyperlink ref="F27" r:id="rId76" tooltip="14. Import ngx-admin theme and styles config in vendor.scss_x000a__x000a_Connecting SCSS files" display="https://github.com/Spirovanni/Pirate-Castle/commit/b82c1fd4f4ea02cceb9f786aac12ea88ac0eb1c9"/>
+    <hyperlink ref="J27" r:id="rId77" tooltip="Merged Pull Request: 14. Import ngx-admin theme and styles config in vendor.scss" display="https://github.com/Spirovanni/Pirate-Castle/pull/14"/>
+    <hyperlink ref="K27" r:id="rId78" display="https://github.com/Spirovanni/Pirate-Castle/commit/d8f32fab62468081b5d66cf40e12068572e4c21f"/>
+    <hyperlink ref="F28" r:id="rId79" tooltip="15. Clear jhipster bootstrap style configs that can conflict with_x000a__x000a_ngx-admin styles" display="https://github.com/Spirovanni/Pirate-Castle/commit/327e5ddc66f329c757c423fef55590b75726dfeb"/>
+    <hyperlink ref="J28" r:id="rId80" tooltip="Merged Pull Request: 15. Clear jhipster bootstrap style configs that can conflict with" display="https://github.com/Spirovanni/Pirate-Castle/pull/15"/>
+    <hyperlink ref="K28" r:id="rId81" display="https://github.com/Spirovanni/Pirate-Castle/commit/b82c1fd4f4ea02cceb9f786aac12ea88ac0eb1c9"/>
+    <hyperlink ref="F29" r:id="rId82" tooltip="17. Echarts dependency install and compnent configs applied._x000a__x000a_npm install echarts@3.7.2 --save;" display="https://github.com/Spirovanni/Pirate-Castle/commit/d481422865fb0045eecc23700b50649ffd1be0db"/>
+    <hyperlink ref="J29" r:id="rId83" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/16"/>
+    <hyperlink ref="K29" r:id="rId84" display="https://github.com/Spirovanni/Pirate-Castle/commit/70338c0506ae76b4d289c0bee4a0b3d96344f399"/>
+    <hyperlink ref="F30" r:id="rId85" tooltip="18. tinymce and chart components js bundle configs" display="https://github.com/Spirovanni/Pirate-Castle/commit/fb44622459762e704b049cc0f3d672a01d5e69a8"/>
+    <hyperlink ref="J30" r:id="rId86" tooltip="Merged Pull Request: 18. tinymce and chart components js bundle configs" display="https://github.com/Spirovanni/Pirate-Castle/pull/17"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId71"/>
-  <drawing r:id="rId72"/>
+  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId87"/>
+  <drawing r:id="rId88"/>
   <tableParts count="1">
-    <tablePart r:id="rId73"/>
+    <tablePart r:id="rId89"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
25b. Corrected Warnings in @theme/components/tiny-mce files
WARNING in ./src/main/webapp/app/ngx-admin/@theme/components/tiny-mce/tiny-mce.component.ts
[20, 14]: Parentheses are required around the parameters of an arrow function definition
</commit_message>
<xml_diff>
--- a/DevTracker.xlsx
+++ b/DevTracker.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="188">
   <si>
     <t>NAME</t>
   </si>
@@ -942,6 +942,138 @@
   </si>
   <si>
     <t>50 changed files</t>
+  </si>
+  <si>
+    <t>24. Corrected Warnings in pages/charts folder</t>
+  </si>
+  <si>
+    <t>#24</t>
+  </si>
+  <si>
+    <t>WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-multiple-xaxis.component.ts
+[16, 64]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-pie.component.ts
+[16, 64]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-radar.component.ts
+[16, 64]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-line.component.ts
+[16, 64]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-bar.component.ts
+[16, 64]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-bar-horizontal.component.ts
+[16, 64]: Parentheses are required around the parameters of an arrow function definition</t>
+  </si>
+  <si>
+    <t>9 changed files</t>
+  </si>
+  <si>
+    <r>
+      <t>147 additions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>224 deletions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>9b2460bfab1deef0ad4a2262cca728baee354eb9</t>
+  </si>
+  <si>
+    <t>1 parent 0df7406</t>
+  </si>
+  <si>
+    <t>0df7406dc2e38e3a4b036b4aabad0d4be6078453</t>
+  </si>
+  <si>
+    <r>
+      <t>424 additions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>742 deletions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>1 parent 9893d85 </t>
+  </si>
+  <si>
+    <t>25. Corrected Warnings in pages/charts/echarts folder</t>
+  </si>
+  <si>
+    <t>WARNING in ./src/main/webapp/app/ngx-admin/pages/ui-features/buttons/hero-buttons/hero-buttons.component.ts
+[16, 71]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-area-stack.component.ts
+[18, 64]: Parentheses are required around the parameters of an arrow function definition
+[5, 13]: The selector of the component "EchartsAreaStackComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-bar.component.ts
+[18, 64]: Parentheses are required around the parameters of an arrow function definition
+[5, 13]: The selector of the component "EchartsBarComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-line.component.ts
+[18, 64]: Parentheses are required around the parameters of an arrow function definition
+[5, 13]: The selector of the component "EchartsLineComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-pie.component.ts
+[18, 64]: Parentheses are required around the parameters of an arrow function definition
+[5, 13]: The selector of the component "EchartsPieComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-radar.component.ts
+[18, 64]: Parentheses are required around the parameters of an arrow function definition
+[5, 13]: The selector of the component "EchartsRadarComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-multiple-xaxis.component.ts
+[18, 64]: Parentheses are required around the parameters of an arrow function definition
+[61, 28]: Parentheses are required around the parameters of an arrow function definition
+[101, 28]: Parentheses are required around the parameters of an arrow function definition
+[5, 13]: The selector of the component "EchartsMultipleXaxisComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-bar-animation.component.ts
+[18, 64]: Parentheses are required around the parameters of an arrow function definition
+ [5, 13]: The selector of the component "EchartsBarAnimationComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)</t>
+  </si>
+  <si>
+    <t>11 changed files</t>
   </si>
 </sst>
 </file>
@@ -3479,8 +3611,8 @@
   </sheetPr>
   <dimension ref="A1:M327"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B30" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -4379,6 +4511,15 @@
       <c r="J36" s="14" t="s">
         <v>173</v>
       </c>
+      <c r="K36" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="L36" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="M36" s="27" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="37" spans="3:13" ht="18" customHeight="1">
       <c r="C37" s="17">
@@ -4390,8 +4531,29 @@
       <c r="E37" s="14" t="s">
         <v>12</v>
       </c>
+      <c r="F37" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="H37" s="32" t="s">
+        <v>178</v>
+      </c>
       <c r="I37" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="L37" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="M37" s="27" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="3:13" ht="18" customHeight="1">
@@ -4404,8 +4566,20 @@
       <c r="E38" s="14" t="s">
         <v>12</v>
       </c>
+      <c r="F38" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="H38" s="32" t="s">
+        <v>187</v>
+      </c>
       <c r="I38" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="3:13" ht="18" customHeight="1">
@@ -5596,19 +5770,19 @@
       <c r="C327" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I41:I55 E14:E55 F37:H55 K36:K55 J37:J55 C13:D55">
+  <conditionalFormatting sqref="I41:I55 E14:E55 C13:D55 F39:F55 H39:H55 G37:G55 K38:K55 J39:J55">
     <cfRule type="expression" dxfId="18" priority="4">
       <formula>#REF!="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="F37:G55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="G37:G55 F39:F55">
       <formula1>Courses</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This employee name isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Personnel Info sheet, it will automatically appear in the list." sqref="E46:E55">
       <formula1>Employees</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="H37:H55 I41:I55 J37:J55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="H39:H55 I41:I55 J39:J55">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5717,13 +5891,19 @@
     <hyperlink ref="K35" r:id="rId102" display="https://github.com/Spirovanni/Pirate-Castle/commit/06e453d6b28e0969123cc65cccd5220f7a7bfab0"/>
     <hyperlink ref="F36" r:id="rId103" tooltip="23. Updated the other files in &quot;@theme/ components &amp; layouts&quot;_x000a__x000a_Replaced &quot;ngx&quot; with &quot;jhi&quot; in selectors." display="https://github.com/Spirovanni/Pirate-Castle/commit/0df7406dc2e38e3a4b036b4aabad0d4be6078453"/>
     <hyperlink ref="J36" r:id="rId104" tooltip="Merged Pull Request: 23. Updated the other files in &quot;@theme/ components &amp; layouts&quot;" display="https://github.com/Spirovanni/Pirate-Castle/pull/23"/>
+    <hyperlink ref="F37" r:id="rId105" tooltip="24. Corrected Warnings in pages/charts folder_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-multiple-xaxis.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-pie.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-radar.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-line.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-bar.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-bar-horizontal.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition" display="https://github.com/Spirovanni/Pirate-Castle/commit/9b2460bfab1deef0ad4a2262cca728baee354eb9"/>
+    <hyperlink ref="J37" r:id="rId106" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/24"/>
+    <hyperlink ref="K37" r:id="rId107" display="https://github.com/Spirovanni/Pirate-Castle/commit/0df7406dc2e38e3a4b036b4aabad0d4be6078453"/>
+    <hyperlink ref="K36" r:id="rId108" display="https://github.com/Spirovanni/Pirate-Castle/commit/9893d85e59b5ee28753c1ae2080bf9cc42011a2e"/>
+    <hyperlink ref="F38" r:id="rId109" tooltip="25. Corrected Warnings in pages/charts/echarts folder_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/ui-features/buttons/hero-buttons/hero-buttons.component.ts_x000a_[16, 71]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-area-stack.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsAreaStackComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-bar.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsBarComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-line.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsLineComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-pie.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsPieComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-radar.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsRadarComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-multiple-xaxis.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[61, 28]: Parentheses are required around the parameters of an arrow function definition_x000a_[101, 28]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsMultipleXaxisComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-bar-animation.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_ [5, 13]: The selector of the component &quot;EchartsBarAnimationComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)" display="https://github.com/Spirovanni/Pirate-Castle/commit/f141dd65d9d4cae1e8b0eea04951a6291cf83e15"/>
+    <hyperlink ref="J38" r:id="rId110" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/24"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId105"/>
-  <drawing r:id="rId106"/>
+  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId111"/>
+  <drawing r:id="rId112"/>
   <tableParts count="1">
-    <tablePart r:id="rId107"/>
+    <tablePart r:id="rId113"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
28. Fixed all broken migration issues
MissionSuccess!!
</commit_message>
<xml_diff>
--- a/DevTracker.xlsx
+++ b/DevTracker.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="207">
   <si>
     <t>NAME</t>
   </si>
@@ -1074,6 +1074,209 @@
   </si>
   <si>
     <t>11 changed files</t>
+  </si>
+  <si>
+    <t>1 parent 9b2460b</t>
+  </si>
+  <si>
+    <t>f141dd65d9d4cae1e8b0eea04951a6291cf83e15</t>
+  </si>
+  <si>
+    <r>
+      <t>132 additions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>125 deletions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>25b. Corrected Warnings in @theme/components/tiny-mce files</t>
+  </si>
+  <si>
+    <t>WARNING in ./src/main/webapp/app/ngx-admin/@theme/components/tiny-mce/tiny-mce.component.ts
+[20, 14]: Parentheses are required around the parameters of an arrow function definition</t>
+  </si>
+  <si>
+    <t>1 parent f141dd6</t>
+  </si>
+  <si>
+    <t>#25</t>
+  </si>
+  <si>
+    <t>46fd768d0688f5522aec5c767af3f2fb840d10fa</t>
+  </si>
+  <si>
+    <r>
+      <t>33 additions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>31 deletions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>26. Corrected Warning in various files </t>
+  </si>
+  <si>
+    <t>WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/dashboard.module.ts
+[23, 1]: Consecutive blank lines are forbidden
+WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/temperature/temperature.component.ts
+[23, 64]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/electricity/electricity.component.ts
+[24, 71]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/traffic/traffic-chart.component.ts
+[26, 73]: Parentheses are required around the parameters of an arrow function definition
+[101, 30]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/d3/d3-pie.component.ts
+[27, 64]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/maps/bubble/bubble-map.component.ts
+[31, 18]: Parentheses are required around the parameters of an arrow function definition
+[471, 24]: Parentheses are required around the parameters of an arrow function definition
+[508, 38]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/d3/d3-advanced-pie.component.ts
+[32, 64]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/traffic/traffic.component.ts
+[34, 71]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts.component.ts
+[4, 13]: The selector of the component "EchartsComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/editors/editors.component.ts
+[4, 13]: The selector of the component "EditorsComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/forms/form-inputs/form-inputs.component.ts
+[4, 13]: The selector of the component "FormInputsComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/forms/form-layouts/form-layouts.component.ts
+[4, 13]: The selector of the component "FormLayoutsComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/forms/forms.component.ts
+[4, 13]: The selector of the component "FormsComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/editors/tiny-mce/tiny-mce.component.ts
+[4, 13]: The selector of the component "TinyMCEComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/@core/core.module.ts
+[41, 3]: Declaration of static method not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/solar/solar.component.ts
+[44, 73]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/electricity/electricity-chart/electricity-chart.component.ts
+[44, 73]: Parentheses are required around the parameters of an arrow function definition
+[79, 33]: Parentheses are required around the parameters of an arrow function definition
+[158, 35]: Parentheses are required around the parameters of an arrow function definition
+[181, 35]: Parentheses are required around the parameters of an arrow function definition
+WARNING in ./src/main/webapp/app/ngx-admin/pages/components/tree/tree.component.ts
+[5, 13]: The selector of the component "TreeComponent" should have prefix "jhi" (https://angular.io/styleguide#style-02-07)
+WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/temperature/temperature-dragger/temperature-dragger.component.ts
+[52, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[53, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[55, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[56, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[57, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[58, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[59, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[60, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[61, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[62, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[63, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[65, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[75, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[76, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface.
+[350, 3]: Declaration of static method not allowed after declaration of instance method. Instead, this should come after instance fields.
+[143, 1]: Consecutive blank lines are forbidden</t>
+  </si>
+  <si>
+    <t>21 changed files</t>
+  </si>
+  <si>
+    <t>#26</t>
+  </si>
+  <si>
+    <t>1 parent 46fd768</t>
+  </si>
+  <si>
+    <t>06e78f523f84a35f073a7b9e7615208f9b8c07c7</t>
+  </si>
+  <si>
+    <r>
+      <t>375 additions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>294 deletions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>27. Fixed last warnings</t>
+  </si>
+  <si>
+    <t>15 changed files</t>
+  </si>
+  <si>
+    <t>#27</t>
   </si>
 </sst>
 </file>
@@ -1345,23 +1548,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="35">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2015,31 +2202,31 @@
   </dxfs>
   <tableStyles count="5" defaultTableStyle="Employee Training Tracker - Log" defaultPivotStyle="PivotTable Style 1">
     <tableStyle name="Employee Training Tracker" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="35"/>
-      <tableStyleElement type="headerRow" dxfId="34"/>
+      <tableStyleElement type="wholeTable" dxfId="34"/>
+      <tableStyleElement type="headerRow" dxfId="33"/>
     </tableStyle>
     <tableStyle name="Employee Training Tracker - Info" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="33"/>
-      <tableStyleElement type="headerRow" dxfId="32"/>
-      <tableStyleElement type="totalRow" dxfId="31"/>
-      <tableStyleElement type="firstColumn" dxfId="30"/>
+      <tableStyleElement type="wholeTable" dxfId="32"/>
+      <tableStyleElement type="headerRow" dxfId="31"/>
+      <tableStyleElement type="totalRow" dxfId="30"/>
+      <tableStyleElement type="firstColumn" dxfId="29"/>
     </tableStyle>
     <tableStyle name="Employee Training Tracker - List" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="29"/>
-      <tableStyleElement type="headerRow" dxfId="28"/>
-      <tableStyleElement type="totalRow" dxfId="27"/>
-      <tableStyleElement type="firstColumn" dxfId="26"/>
+      <tableStyleElement type="wholeTable" dxfId="28"/>
+      <tableStyleElement type="headerRow" dxfId="27"/>
+      <tableStyleElement type="totalRow" dxfId="26"/>
+      <tableStyleElement type="firstColumn" dxfId="25"/>
     </tableStyle>
     <tableStyle name="Employee Training Tracker - Log" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="25"/>
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="totalRow" dxfId="23"/>
-      <tableStyleElement type="firstColumn" dxfId="22"/>
+      <tableStyleElement type="wholeTable" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="totalRow" dxfId="22"/>
+      <tableStyleElement type="firstColumn" dxfId="21"/>
     </tableStyle>
     <tableStyle name="PivotTable Style 1" table="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="21"/>
-      <tableStyleElement type="headerRow" dxfId="20"/>
-      <tableStyleElement type="firstColumn" dxfId="19"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="firstColumn" dxfId="18"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -3332,8 +3519,8 @@
     <filterColumn colId="10"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="4" name="DATE OF COMMIT" dataDxfId="17"/>
-    <tableColumn id="3" name="TIME" dataDxfId="16"/>
+    <tableColumn id="4" name="DATE OF COMMIT" dataDxfId="16"/>
+    <tableColumn id="3" name="TIME" dataDxfId="15"/>
     <tableColumn id="1" name="DEVELOPER"/>
     <tableColumn id="2" name="FEATURE"/>
     <tableColumn id="5" name="DETAILS"/>
@@ -3355,24 +3542,24 @@
   </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" name="FEATURE"/>
-    <tableColumn id="2" name="DESCRIPTION" dataDxfId="14"/>
-    <tableColumn id="3" name="FILE" dataDxfId="13"/>
-    <tableColumn id="4" name="HOURS" dataDxfId="12"/>
+    <tableColumn id="2" name="DESCRIPTION" dataDxfId="13"/>
+    <tableColumn id="3" name="FILE" dataDxfId="12"/>
+    <tableColumn id="4" name="HOURS" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="Employee Training Tracker - List" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEmployeeInfo" displayName="tblEmployeeInfo" ref="C5:F50" totalsRowShown="0" dataDxfId="10" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEmployeeInfo" displayName="tblEmployeeInfo" ref="C5:F50" totalsRowShown="0" dataDxfId="9" headerRowCellStyle="Heading 2">
   <autoFilter ref="C5:F50">
     <filterColumn colId="2"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="NAME" dataDxfId="9"/>
-    <tableColumn id="2" name="Department" dataDxfId="8"/>
-    <tableColumn id="4" name="Title" dataDxfId="7"/>
-    <tableColumn id="3" name="HOURS" dataDxfId="6"/>
+    <tableColumn id="1" name="NAME" dataDxfId="8"/>
+    <tableColumn id="2" name="Department" dataDxfId="7"/>
+    <tableColumn id="4" name="Title" dataDxfId="6"/>
+    <tableColumn id="3" name="HOURS" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Employee Training Tracker - Info" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3611,8 +3798,8 @@
   </sheetPr>
   <dimension ref="A1:M327"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C35" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -4526,7 +4713,7 @@
         <v>43142</v>
       </c>
       <c r="D37" s="15">
-        <v>2.2916666666666669E-2</v>
+        <v>0.57152777777777775</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>12</v>
@@ -4561,7 +4748,7 @@
         <v>43142</v>
       </c>
       <c r="D38" s="15">
-        <v>2.2916666666666669E-2</v>
+        <v>0.62361111111111112</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>12</v>
@@ -4580,6 +4767,15 @@
       </c>
       <c r="J38" s="14" t="s">
         <v>176</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="L38" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="M38" s="27" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="3:13" ht="18" customHeight="1">
@@ -4587,13 +4783,34 @@
         <v>43142</v>
       </c>
       <c r="D39" s="15">
-        <v>2.2916666666666669E-2</v>
+        <v>0.65833333333333333</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>12</v>
       </c>
+      <c r="F39" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="H39" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="I39" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="L39" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="3:13" ht="18" customHeight="1">
@@ -4601,13 +4818,34 @@
         <v>43142</v>
       </c>
       <c r="D40" s="15">
-        <v>2.2916666666666669E-2</v>
+        <v>0.81111111111111101</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>12</v>
       </c>
+      <c r="F40" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="H40" s="32" t="s">
+        <v>199</v>
+      </c>
       <c r="I40" s="14" t="s">
         <v>18</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="L40" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="M40" s="27" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="3:13" ht="18" customHeight="1">
@@ -4615,10 +4853,19 @@
         <v>43142</v>
       </c>
       <c r="D41" s="15">
-        <v>2.2916666666666669E-2</v>
+        <v>0.56111111111111112</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>12</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="3:13" ht="18" customHeight="1">
@@ -5770,19 +6017,19 @@
       <c r="C327" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I41:I55 E14:E55 C13:D55 F39:F55 H39:H55 G37:G55 K38:K55 J39:J55">
-    <cfRule type="expression" dxfId="18" priority="4">
+  <conditionalFormatting sqref="E14:E55 C13:D55 G37:G55 F42:F55 H42:H55 I41:I55 K41:K55 J42:J55">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>#REF!="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="G37:G55 F39:F55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="G37:G55 F42:F55">
       <formula1>Courses</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This employee name isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Personnel Info sheet, it will automatically appear in the list." sqref="E46:E55">
       <formula1>Employees</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="H39:H55 I41:I55 J39:J55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="H42:H55 I41:I55 J42:J55">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5897,13 +6144,22 @@
     <hyperlink ref="K36" r:id="rId108" display="https://github.com/Spirovanni/Pirate-Castle/commit/9893d85e59b5ee28753c1ae2080bf9cc42011a2e"/>
     <hyperlink ref="F38" r:id="rId109" tooltip="25. Corrected Warnings in pages/charts/echarts folder_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/ui-features/buttons/hero-buttons/hero-buttons.component.ts_x000a_[16, 71]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-area-stack.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsAreaStackComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-bar.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsBarComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-line.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsLineComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-pie.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsPieComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-radar.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsRadarComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-multiple-xaxis.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[61, 28]: Parentheses are required around the parameters of an arrow function definition_x000a_[101, 28]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsMultipleXaxisComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-bar-animation.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_ [5, 13]: The selector of the component &quot;EchartsBarAnimationComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)" display="https://github.com/Spirovanni/Pirate-Castle/commit/f141dd65d9d4cae1e8b0eea04951a6291cf83e15"/>
     <hyperlink ref="J38" r:id="rId110" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/24"/>
+    <hyperlink ref="K38" r:id="rId111" display="https://github.com/Spirovanni/Pirate-Castle/commit/9b2460bfab1deef0ad4a2262cca728baee354eb9"/>
+    <hyperlink ref="F39" r:id="rId112" tooltip="25b. Corrected Warnings in @theme/components/tiny-mce files_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/@theme/components/tiny-mce/tiny-mce.component.ts_x000a_[20, 14]: Parentheses are required around the parameters of an arrow function definition" display="https://github.com/Spirovanni/Pirate-Castle/commit/46fd768d0688f5522aec5c767af3f2fb840d10fa"/>
+    <hyperlink ref="K39" r:id="rId113" display="https://github.com/Spirovanni/Pirate-Castle/commit/f141dd65d9d4cae1e8b0eea04951a6291cf83e15"/>
+    <hyperlink ref="J39" r:id="rId114" tooltip="Merged Pull Request: 25b. Corrected Warnings in @theme/components/tiny-mce files" display="https://github.com/Spirovanni/Pirate-Castle/pull/25"/>
+    <hyperlink ref="F40" r:id="rId115" tooltip="26. Corrected Warning in various files_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/dashboard.module.ts_x000a_[23, 1]: Consecutive blank lines are forbidden_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/temperature/temperature.component.ts_x000a_[23, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/electricity/electricity.component.ts_x000a_[24, 71]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/traffic/traffic-chart.component.ts_x000a_[26, 73]: Parentheses are required around the parameters of an arrow function definition_x000a_[101, 30]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/d3/d3-pie.component.ts_x000a_[27, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/maps/bubble/bubble-map.component.ts_x000a_[31, 18]: Parentheses are required around the parameters of an arrow function definition_x000a_[471, 24]: Parentheses are required around the parameters of an arrow function definition_x000a_[508, 38]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/d3/d3-advanced-pie.component.ts_x000a_[32, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/traffic/traffic.component.ts_x000a_[34, 71]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts.component.ts_x000a_[4, 13]: The selector of the component &quot;EchartsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/editors/editors.component.ts_x000a_[4, 13]: The selector of the component &quot;EditorsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/forms/form-inputs/form-inputs.component.ts_x000a_[4, 13]: The selector of the component &quot;FormInputsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/forms/form-layouts/form-layouts.component.ts_x000a_[4, 13]: The selector of the component &quot;FormLayoutsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/forms/forms.component.ts_x000a_[4, 13]: The selector of the component &quot;FormsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/editors/tiny-mce/tiny-mce.component.ts_x000a_[4, 13]: The selector of the component &quot;TinyMCEComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/@core/core.module.ts_x000a_[41, 3]: Declaration of static method not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/solar/solar.component.ts_x000a_[44, 73]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/electricity/electricity-chart/electricity-chart.component.ts_x000a_[44, 73]: Parentheses are required around the parameters of an arrow function definition_x000a_[79, 33]: Parentheses are required around the parameters of an arrow function definition_x000a_[158, 35]: Parentheses are required around the parameters of an arrow function definition_x000a_[181, 35]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/components/tree/tree.component.ts_x000a_[5, 13]: The selector of the component &quot;TreeComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/temperature/temperature-dragger/temperature-dragger.component.ts_x000a_[52, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[53, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[55, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[56, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[57, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[58, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[59, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[60, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[61, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[62, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[63, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[65, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[75, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[76, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[350, 3]: Declaration of static method not allowed after declaration of instance method. Instead, this should come after instance fields._x000a_[143, 1]: Consecutive blank lines are forbidden" display="https://github.com/Spirovanni/Pirate-Castle/commit/06e78f523f84a35f073a7b9e7615208f9b8c07c7"/>
+    <hyperlink ref="J40" r:id="rId116" tooltip="Merged Pull Request: 26. Corrected Warning in various files" display="https://github.com/Spirovanni/Pirate-Castle/pull/26"/>
+    <hyperlink ref="K40" r:id="rId117" display="https://github.com/Spirovanni/Pirate-Castle/commit/46fd768d0688f5522aec5c767af3f2fb840d10fa"/>
+    <hyperlink ref="F41" r:id="rId118" tooltip="27. Fixed last warnings_x000a__x000a_Ran without warnings" display="https://github.com/Spirovanni/Pirate-Castle/commit/535df5af0e73b859e37a4f1accd7af8008d3a3ce"/>
+    <hyperlink ref="J41" r:id="rId119" tooltip="Merged Pull Request: 27. Fixed last warnings" display="https://github.com/Spirovanni/Pirate-Castle/pull/27"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId111"/>
-  <drawing r:id="rId112"/>
+  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId120"/>
+  <drawing r:id="rId121"/>
   <tableParts count="1">
-    <tablePart r:id="rId113"/>
+    <tablePart r:id="rId122"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6083,7 +6339,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:C30 F6:F30">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>COUNTIF($C:$C,$C6)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6460,7 +6716,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:G50">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>(COUNTIF($C:$C,$C6)&gt;1)*($C6&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
33. Attempting to connect features in Header
Added Logo style
</commit_message>
<xml_diff>
--- a/DevTracker.xlsx
+++ b/DevTracker.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="219">
   <si>
     <t>NAME</t>
   </si>
@@ -296,62 +296,6 @@
 and import it in app-module</t>
   </si>
   <si>
-    <r>
-      <t>6 changed files</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>3 changed files</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>2 changed files</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
     <t>8 changed files </t>
   </si>
   <si>
@@ -379,20 +323,6 @@
     <t>#10</t>
   </si>
   <si>
-    <r>
-      <t>3 changed files</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
     <t>1 parent 5d289bf</t>
   </si>
   <si>
@@ -429,27 +359,6 @@
     <t>…et web folder to be able to served from application</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>4 changed files</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
     <t>#12</t>
   </si>
   <si>
@@ -480,38 +389,6 @@
     <t>d8f32fab62468081b5d66cf40e12068572e4c21f</t>
   </si>
   <si>
-    <r>
-      <t>28 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>56 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>14. Import ngx-admin theme and styles config in vendor.scss</t>
   </si>
   <si>
@@ -530,38 +407,6 @@
     <t>b82c1fd4f4ea02cceb9f786aac12ea88ac0eb1c9</t>
   </si>
   <si>
-    <r>
-      <t>54 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>24 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>15. Clear jhipster bootstrap style configs that can conflict with</t>
   </si>
   <si>
@@ -577,38 +422,6 @@
     <t>327e5ddc66f329c757c423fef55590b75726dfeb</t>
   </si>
   <si>
-    <r>
-      <t>54 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>292 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>6 changed files</t>
   </si>
   <si>
@@ -624,38 +437,6 @@
     <t>d481422865fb0045eecc23700b50649ffd1be0db</t>
   </si>
   <si>
-    <r>
-      <t>87 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>36 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>#17</t>
   </si>
   <si>
@@ -671,38 +452,6 @@
     <t>fb44622459762e704b049cc0f3d672a01d5e69a8</t>
   </si>
   <si>
-    <r>
-      <t>44 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>59 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>18. String based lazy router loading fixes.</t>
   </si>
   <si>
@@ -715,38 +464,6 @@
     <t>6cef9c251affc1695a2b4bda5a3fa66ac419a283</t>
   </si>
   <si>
-    <r>
-      <t>67 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>26 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>19. Echarts world component js added </t>
   </si>
   <si>
@@ -759,38 +476,6 @@
     <t>3628054f0bfea6114f7867d8febf92d3ca38ca0f</t>
   </si>
   <si>
-    <r>
-      <t>17 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>18 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>20. Adding Doc folder </t>
   </si>
   <si>
@@ -800,38 +485,6 @@
     <t>#20</t>
   </si>
   <si>
-    <r>
-      <t>88 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>100 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>4187afd07e808429beb3e235e4bc8bff6758e488</t>
   </si>
   <si>
@@ -856,38 +509,6 @@
     <t>06e453d6b28e0969123cc65cccd5220f7a7bfab0</t>
   </si>
   <si>
-    <r>
-      <t>562 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>129 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>22. Update "@theme/ components &amp; layouts"</t>
   </si>
   <si>
@@ -901,38 +522,6 @@
   </si>
   <si>
     <t>9893d85e59b5ee28753c1ae2080bf9cc42011a2e</t>
-  </si>
-  <si>
-    <r>
-      <t>535 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>28,291 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <t>23. Updated the other files in "@theme/ components &amp; layouts"</t>
@@ -967,38 +556,6 @@
     <t>9 changed files</t>
   </si>
   <si>
-    <r>
-      <t>147 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>224 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>9b2460bfab1deef0ad4a2262cca728baee354eb9</t>
   </si>
   <si>
@@ -1006,38 +563,6 @@
   </si>
   <si>
     <t>0df7406dc2e38e3a4b036b4aabad0d4be6078453</t>
-  </si>
-  <si>
-    <r>
-      <t>424 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>742 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <t>1 parent 9893d85 </t>
@@ -1082,38 +607,6 @@
     <t>f141dd65d9d4cae1e8b0eea04951a6291cf83e15</t>
   </si>
   <si>
-    <r>
-      <t>132 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>125 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>25b. Corrected Warnings in @theme/components/tiny-mce files</t>
   </si>
   <si>
@@ -1128,38 +621,6 @@
   </si>
   <si>
     <t>46fd768d0688f5522aec5c767af3f2fb840d10fa</t>
-  </si>
-  <si>
-    <r>
-      <t>33 additions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>31 deletions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF24292E"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <t>26. Corrected Warning in various files </t>
@@ -1238,8 +699,119 @@
     <t>06e78f523f84a35f073a7b9e7615208f9b8c07c7</t>
   </si>
   <si>
+    <t>27. Fixed last warnings</t>
+  </si>
+  <si>
+    <t>15 changed files</t>
+  </si>
+  <si>
+    <t>#27</t>
+  </si>
+  <si>
+    <t>Ran without warnings</t>
+  </si>
+  <si>
+    <t>1 parent 06e78f5</t>
+  </si>
+  <si>
+    <t>535df5af0e73b859e37a4f1accd7af8008d3a3ce</t>
+  </si>
+  <si>
+    <t>28 additions and 56 deletions.</t>
+  </si>
+  <si>
+    <t>54 additions and 24 deletions.</t>
+  </si>
+  <si>
+    <t>54 additions and 292 deletions.</t>
+  </si>
+  <si>
+    <t>87 additions and 36 deletions.</t>
+  </si>
+  <si>
+    <t>44 additions and 59 deletions.</t>
+  </si>
+  <si>
+    <t>67 additions and 26 deletions.</t>
+  </si>
+  <si>
+    <t>17 additions and 18 deletions.</t>
+  </si>
+  <si>
+    <t>88 additions and 100 deletions.</t>
+  </si>
+  <si>
+    <t>562 additions and 129 deletions.</t>
+  </si>
+  <si>
+    <t>535 additions and 28,291 deletions.</t>
+  </si>
+  <si>
+    <t>424 additions and 742 deletions.</t>
+  </si>
+  <si>
+    <t>2 changed files </t>
+  </si>
+  <si>
+    <t>3 changed files </t>
+  </si>
+  <si>
+    <t>6 changed files </t>
+  </si>
+  <si>
+    <t>4 changed files </t>
+  </si>
+  <si>
+    <t>147 additions and 224 deletions.</t>
+  </si>
+  <si>
+    <t>132 additions and 125 deletions.</t>
+  </si>
+  <si>
+    <t>33 additions and 31 deletions.</t>
+  </si>
+  <si>
+    <t>375 additions and 294 deletions.</t>
+  </si>
+  <si>
+    <t>342 additions and 430 deletions.</t>
+  </si>
+  <si>
+    <t>29. Switched to "jhi-main" in index.html </t>
+  </si>
+  <si>
+    <t>28. Fixed all broken migration issues</t>
+  </si>
+  <si>
+    <t>Attempting to use original infastructure.</t>
+  </si>
+  <si>
     <r>
-      <t>375 additions</t>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>6 changed files</t>
+    </r>
+  </si>
+  <si>
+    <t>#29</t>
+  </si>
+  <si>
+    <t>1 parent 2fec5c3</t>
+  </si>
+  <si>
+    <t>c3d9fc338ad245a0fde711a23669ef6cef73129d</t>
+  </si>
+  <si>
+    <r>
+      <t>327 additions</t>
     </r>
     <r>
       <rPr>
@@ -1257,7 +829,7 @@
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
-      <t>294 deletions</t>
+      <t>209 deletions</t>
     </r>
     <r>
       <rPr>
@@ -1270,13 +842,7 @@
     </r>
   </si>
   <si>
-    <t>27. Fixed last warnings</t>
-  </si>
-  <si>
-    <t>15 changed files</t>
-  </si>
-  <si>
-    <t>#27</t>
+    <t>MissionSuccess!!</t>
   </si>
 </sst>
 </file>
@@ -1286,7 +852,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="12">
     <font>
       <sz val="9"/>
       <color theme="1" tint="0.499984740745262"/>
@@ -1330,12 +896,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF05264C"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF444D56"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -1347,19 +907,7 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF444D56"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Segoe UI Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
+      <sz val="11"/>
       <color rgb="FF24292E"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -1371,31 +919,19 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1" tint="0.499984740745262"/>
+      <sz val="9"/>
+      <color theme="1" tint="0.249977111117893"/>
       <name val="Century Gothic"/>
       <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF24292E"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Segoe UI Light"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color rgb="FF0366D6"/>
-      <name val="Segoe UI"/>
+      <sz val="9"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Century Gothic"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1443,7 +979,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1499,46 +1035,43 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="11" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1548,87 +1081,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="35">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <font>
         <b val="0"/>
@@ -2202,31 +1655,31 @@
   </dxfs>
   <tableStyles count="5" defaultTableStyle="Employee Training Tracker - Log" defaultPivotStyle="PivotTable Style 1">
     <tableStyle name="Employee Training Tracker" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="34"/>
-      <tableStyleElement type="headerRow" dxfId="33"/>
+      <tableStyleElement type="wholeTable" dxfId="29"/>
+      <tableStyleElement type="headerRow" dxfId="28"/>
     </tableStyle>
     <tableStyle name="Employee Training Tracker - Info" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="32"/>
-      <tableStyleElement type="headerRow" dxfId="31"/>
-      <tableStyleElement type="totalRow" dxfId="30"/>
-      <tableStyleElement type="firstColumn" dxfId="29"/>
+      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="totalRow" dxfId="25"/>
+      <tableStyleElement type="firstColumn" dxfId="24"/>
     </tableStyle>
     <tableStyle name="Employee Training Tracker - List" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="28"/>
-      <tableStyleElement type="headerRow" dxfId="27"/>
-      <tableStyleElement type="totalRow" dxfId="26"/>
-      <tableStyleElement type="firstColumn" dxfId="25"/>
+      <tableStyleElement type="wholeTable" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="22"/>
+      <tableStyleElement type="totalRow" dxfId="21"/>
+      <tableStyleElement type="firstColumn" dxfId="20"/>
     </tableStyle>
     <tableStyle name="Employee Training Tracker - Log" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="24"/>
-      <tableStyleElement type="headerRow" dxfId="23"/>
-      <tableStyleElement type="totalRow" dxfId="22"/>
-      <tableStyleElement type="firstColumn" dxfId="21"/>
+      <tableStyleElement type="wholeTable" dxfId="19"/>
+      <tableStyleElement type="headerRow" dxfId="18"/>
+      <tableStyleElement type="totalRow" dxfId="17"/>
+      <tableStyleElement type="firstColumn" dxfId="16"/>
     </tableStyle>
     <tableStyle name="PivotTable Style 1" table="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="firstColumn" dxfId="18"/>
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -2252,7 +1705,7 @@
         <xdr:cNvPr id="5" name="Training Log" descr="&quot;&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2351,7 +1804,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Click to view Course List"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2431,7 +1884,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2" tooltip="Click to view Personal Info"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2519,7 +1972,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2" descr="&quot;&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2580,7 +2033,7 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns="" Requires="sle15">
+      <mc:Choice xmlns="" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="14" name="NAME" descr="Click a name in the Slicer to filter the Training Log by your selection. " title="Name Slicer">
@@ -2658,7 +2111,7 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns="" Requires="sle15">
+      <mc:Choice xmlns="" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="15" name="COURSE" descr="Click a course in the Slicer to filter the Training Log by your selection. " title="Course Slicer">
@@ -2736,7 +2189,7 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns="" Requires="sle15">
+      <mc:Choice xmlns="" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="17" name="TAKEN" descr="Click an entry in the Slicer to filter the Training Log by your selection. " title="Taken Slicer">
@@ -2824,7 +2277,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Click to view Training Log"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2903,7 +2356,7 @@
         <xdr:cNvPr id="7" name="Course List" descr="&quot;&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3005,7 +2458,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2" tooltip="Click to view Personal Info"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3084,7 +2537,7 @@
         <xdr:cNvPr id="2" name="Tip" descr="To help make sure each course is listed once, duplicate course titles will display in Red. &#10;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3232,7 +2685,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Click to view Training Log"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3312,7 +2765,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2" tooltip="Click to view Course List"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3391,7 +2844,7 @@
         <xdr:cNvPr id="8" name="Personnel Info" descr="&quot;&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3458,7 +2911,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8" descr="&quot;&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3519,8 +2972,8 @@
     <filterColumn colId="10"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="4" name="DATE OF COMMIT" dataDxfId="16"/>
-    <tableColumn id="3" name="TIME" dataDxfId="15"/>
+    <tableColumn id="4" name="DATE OF COMMIT" dataDxfId="11"/>
+    <tableColumn id="3" name="TIME" dataDxfId="10"/>
     <tableColumn id="1" name="DEVELOPER"/>
     <tableColumn id="2" name="FEATURE"/>
     <tableColumn id="5" name="DETAILS"/>
@@ -3542,24 +2995,24 @@
   </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" name="FEATURE"/>
-    <tableColumn id="2" name="DESCRIPTION" dataDxfId="13"/>
-    <tableColumn id="3" name="FILE" dataDxfId="12"/>
-    <tableColumn id="4" name="HOURS" dataDxfId="11"/>
+    <tableColumn id="2" name="DESCRIPTION" dataDxfId="8"/>
+    <tableColumn id="3" name="FILE" dataDxfId="7"/>
+    <tableColumn id="4" name="HOURS" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Employee Training Tracker - List" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEmployeeInfo" displayName="tblEmployeeInfo" ref="C5:F50" totalsRowShown="0" dataDxfId="9" headerRowCellStyle="Heading 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblEmployeeInfo" displayName="tblEmployeeInfo" ref="C5:F50" totalsRowShown="0" dataDxfId="4" headerRowCellStyle="Heading 2">
   <autoFilter ref="C5:F50">
     <filterColumn colId="2"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="NAME" dataDxfId="8"/>
-    <tableColumn id="2" name="Department" dataDxfId="7"/>
-    <tableColumn id="4" name="Title" dataDxfId="6"/>
-    <tableColumn id="3" name="HOURS" dataDxfId="5"/>
+    <tableColumn id="1" name="NAME" dataDxfId="3"/>
+    <tableColumn id="2" name="Department" dataDxfId="2"/>
+    <tableColumn id="4" name="Title" dataDxfId="1"/>
+    <tableColumn id="3" name="HOURS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Employee Training Tracker - Info" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3798,8 +3251,8 @@
   </sheetPr>
   <dimension ref="A1:M327"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C35" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B34" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -3810,7 +3263,7 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1"/>
+    <col min="7" max="7" width="51.42578125" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" customWidth="1"/>
     <col min="10" max="10" width="6.42578125" customWidth="1"/>
@@ -3872,223 +3325,224 @@
       </c>
     </row>
     <row r="13" spans="3:13" ht="18" customHeight="1">
-      <c r="C13" s="17">
+      <c r="C13" s="23">
         <v>43141</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="24">
         <v>0.67013888888888884</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="I13" s="14" t="s">
+      <c r="H13" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="21" t="s">
+      <c r="L13" s="26" t="s">
         <v>23</v>
       </c>
+      <c r="M13" s="26"/>
     </row>
     <row r="14" spans="3:13" ht="18" customHeight="1">
-      <c r="C14" s="17">
+      <c r="C14" s="23">
         <v>43141</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="24">
         <v>0.68402777777777779</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="L14" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="M14" s="24" t="s">
+      <c r="M14" s="26" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="3:13" ht="21" customHeight="1">
-      <c r="C15" s="17">
+      <c r="C15" s="23">
         <v>43141</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="24">
         <v>0.69374999999999998</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="K15" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="21" t="s">
+      <c r="L15" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="24" t="s">
+      <c r="M15" s="26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="3:13" ht="18" customHeight="1">
-      <c r="C16" s="17">
+      <c r="C16" s="23">
         <v>43141</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="24">
         <v>0.72152777777777777</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="28" t="s">
         <v>34</v>
       </c>
       <c r="H16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="21" t="s">
+      <c r="L16" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="M16" s="24" t="s">
+      <c r="M16" s="26" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="17" spans="3:13" ht="18" customHeight="1">
-      <c r="C17" s="17">
+      <c r="C17" s="23">
         <v>43141</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="24">
         <v>0.78402777777777777</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="30" t="s">
         <v>39</v>
       </c>
       <c r="H17" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="L17" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="M17" s="24" t="s">
+      <c r="M17" s="26" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="3:13" ht="18" customHeight="1">
-      <c r="C18" s="17">
+      <c r="C18" s="23">
         <v>43141</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="24">
         <v>0.81597222222222221</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="30" t="s">
         <v>44</v>
       </c>
       <c r="H18" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="I18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="K18" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="L18" s="21" t="s">
+      <c r="L18" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="M18" s="24" t="s">
+      <c r="M18" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="3:13" ht="18" customHeight="1">
-      <c r="C19" s="17">
+      <c r="C19" s="23">
         <v>43141</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="24">
         <v>0.87083333333333324</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="25" t="s">
         <v>71</v>
       </c>
       <c r="G19" s="28" t="s">
@@ -4097,838 +3551,880 @@
       <c r="H19" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="L19" s="21" t="s">
+      <c r="L19" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="M19" s="24" t="s">
+      <c r="M19" s="26" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="3:13" ht="18" customHeight="1">
-      <c r="C20" s="17">
+      <c r="C20" s="23">
         <v>43141</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="24">
         <v>0.8881944444444444</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="I20" s="14" t="s">
+      <c r="H20" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="I20" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="L20" s="21" t="s">
+      <c r="L20" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="M20" s="24" t="s">
+      <c r="M20" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="3:13" ht="18" customHeight="1">
-      <c r="C21" s="17">
+      <c r="C21" s="23">
         <v>43141</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="24">
         <v>0.92847222222222225</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="30" t="s">
         <v>74</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="I21" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="K21" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="L21" s="21" t="s">
+      <c r="L21" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="M21" s="24" t="s">
+      <c r="M21" s="26" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="3:13" ht="18" customHeight="1">
-      <c r="C22" s="17">
+      <c r="C22" s="23">
         <v>43141</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="24">
         <v>0.94097222222222221</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="25" t="s">
         <v>79</v>
       </c>
       <c r="G22" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="H22" t="s">
-        <v>81</v>
-      </c>
-      <c r="I22" s="14" t="s">
+      <c r="H22" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="I22" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="M22" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K22" s="14" t="s">
+    </row>
+    <row r="23" spans="3:13" ht="18" customHeight="1">
+      <c r="C23" s="23">
+        <v>43141</v>
+      </c>
+      <c r="D23" s="24">
+        <v>0.94444444444444453</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="L22" s="21" t="s">
+      <c r="G23" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="M22" s="24" t="s">
+      <c r="H23" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="25" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="3:13" ht="18" customHeight="1">
-      <c r="C23" s="17">
+      <c r="K23" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="M23" s="26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" ht="18" customHeight="1">
+      <c r="C24" s="23">
         <v>43141</v>
       </c>
-      <c r="D23" s="15">
-        <v>0.94444444444444453</v>
-      </c>
-      <c r="E23" s="14" t="s">
+      <c r="D24" s="24">
+        <v>0.95277777777777783</v>
+      </c>
+      <c r="E24" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="F24" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="G24" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="K23" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="L23" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="M23" s="24" t="s">
+      <c r="J24" s="25" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="3:13" ht="18" customHeight="1">
-      <c r="C24" s="17">
+      <c r="K24" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="L24" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="M24" s="26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" ht="18" customHeight="1">
+      <c r="C25" s="23">
         <v>43141</v>
       </c>
-      <c r="D24" s="15">
-        <v>0.95277777777777783</v>
-      </c>
-      <c r="E24" s="14" t="s">
+      <c r="D25" s="24">
+        <v>0.97430555555555554</v>
+      </c>
+      <c r="E25" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" t="s">
-        <v>99</v>
-      </c>
-      <c r="I24" s="14" t="s">
+      <c r="F25" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="I25" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="L24" s="31" t="s">
+      <c r="J25" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="M24" s="24" t="s">
+      <c r="K25" s="25" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="25" spans="3:13" ht="18" customHeight="1">
-      <c r="C25" s="17">
+      <c r="L25" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="M25" s="26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" ht="18" customHeight="1">
+      <c r="C26" s="23">
         <v>43141</v>
       </c>
-      <c r="D25" s="15">
-        <v>0.97430555555555554</v>
-      </c>
-      <c r="E25" s="14" t="s">
+      <c r="D26" s="24">
+        <v>0.98749999999999993</v>
+      </c>
+      <c r="E26" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="G25" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="H25" s="26" t="s">
+      <c r="F26" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="G26" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="H26" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="I26" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="K25" s="14" t="s">
+      <c r="J26" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="L26" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="M26" s="26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" ht="18" customHeight="1">
+      <c r="C27" s="23">
+        <v>43141</v>
+      </c>
+      <c r="D27" s="24">
+        <v>0.99236111111111114</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="L27" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="M27" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" ht="18" customHeight="1">
+      <c r="C28" s="23">
+        <v>43142</v>
+      </c>
+      <c r="D28" s="24">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G28" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="H28" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="L25" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="M25" s="24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13" ht="18" customHeight="1">
-      <c r="C26" s="17">
-        <v>43141</v>
-      </c>
-      <c r="D26" s="15">
-        <v>0.98749999999999993</v>
-      </c>
-      <c r="E26" s="14" t="s">
+      <c r="I28" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="L28" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="M28" s="26" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" ht="18" customHeight="1">
+      <c r="C29" s="23">
+        <v>43142</v>
+      </c>
+      <c r="D29" s="24">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="E29" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="H26" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="I26" s="14" t="s">
+      <c r="F29" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="J29" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="L29" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="M29" s="26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" ht="18" customHeight="1">
+      <c r="C30" s="23">
+        <v>43142</v>
+      </c>
+      <c r="D30" s="24">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="K26" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="M26" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" ht="18" customHeight="1">
-      <c r="C27" s="17">
-        <v>43141</v>
-      </c>
-      <c r="D27" s="15">
-        <v>0.99236111111111114</v>
-      </c>
-      <c r="E27" s="14" t="s">
+      <c r="I30" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="K30" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="L30" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="M30" s="26" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" ht="18" customHeight="1">
+      <c r="C31" s="23">
+        <v>43142</v>
+      </c>
+      <c r="D31" s="24">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="E31" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="H27" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="I27" s="14" t="s">
+      <c r="F31" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="I31" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J27" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="L27" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="M27" s="27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="3:13" ht="18" customHeight="1">
-      <c r="C28" s="17">
+      <c r="J31" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="K31" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="L31" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="M31" s="26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" ht="18" customHeight="1">
+      <c r="C32" s="23">
         <v>43142</v>
       </c>
-      <c r="D28" s="15">
-        <v>2.0833333333333333E-3</v>
-      </c>
-      <c r="E28" s="14" t="s">
+      <c r="D32" s="24">
+        <v>5.4166666666666669E-2</v>
+      </c>
+      <c r="E32" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="H28" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="I28" s="14" t="s">
+      <c r="F32" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G32" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="I32" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J28" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="L28" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="M28" s="27" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="3:13" ht="18" customHeight="1">
-      <c r="C29" s="17">
+      <c r="J32" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="K32" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="L32" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="M32" s="26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" ht="18" customHeight="1">
+      <c r="C33" s="23">
         <v>43142</v>
       </c>
-      <c r="D29" s="15">
-        <v>1.1805555555555555E-2</v>
-      </c>
-      <c r="E29" s="14" t="s">
+      <c r="D33" s="24">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="E33" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="H29" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="I29" s="14" t="s">
+      <c r="F33" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="I33" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="K29" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="L29" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="M29" s="27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="3:13" ht="18" customHeight="1">
-      <c r="C30" s="17">
+      <c r="J33" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="K33" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="L33" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="M33" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13" ht="18" customHeight="1">
+      <c r="C34" s="23">
         <v>43142</v>
       </c>
-      <c r="D30" s="15">
-        <v>2.2916666666666669E-2</v>
-      </c>
-      <c r="E30" s="14" t="s">
+      <c r="D34" s="24">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="E34" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="I30" s="14" t="s">
+      <c r="F34" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="H34" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="I34" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="L30" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="M30" s="27" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="3:13" ht="18" customHeight="1">
-      <c r="C31" s="17">
+      <c r="J34" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="K34" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="L34" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="M34" s="26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13" ht="18" customHeight="1">
+      <c r="C35" s="23">
         <v>43142</v>
       </c>
-      <c r="D31" s="15">
-        <v>4.6527777777777779E-2</v>
-      </c>
-      <c r="E31" s="14" t="s">
+      <c r="D35" s="24">
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="E35" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="I31" s="14" t="s">
+      <c r="F35" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="I35" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J31" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="K31" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="L31" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="M31" s="27" t="s">
+      <c r="J35" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="K35" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="L35" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="M35" s="26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="3:13" ht="18" customHeight="1">
+      <c r="C36" s="23">
+        <v>43142</v>
+      </c>
+      <c r="D36" s="24">
+        <v>0.56111111111111112</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="G36" s="30" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="32" spans="3:13" ht="18" customHeight="1">
-      <c r="C32" s="17">
+      <c r="H36" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="I36" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="K36" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="L36" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="M36" s="26" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13" ht="18" customHeight="1">
+      <c r="C37" s="23">
         <v>43142</v>
       </c>
-      <c r="D32" s="15">
-        <v>5.4166666666666669E-2</v>
-      </c>
-      <c r="E32" s="14" t="s">
+      <c r="D37" s="24">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="E37" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="I32" s="14" t="s">
+      <c r="F37" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="I37" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="K32" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="L32" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="M32" s="27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="3:13" ht="18" customHeight="1">
-      <c r="C33" s="17">
+      <c r="J37" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="K37" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="L37" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="M37" s="26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13" ht="18" customHeight="1">
+      <c r="C38" s="23">
         <v>43142</v>
       </c>
-      <c r="D33" s="15">
-        <v>6.1111111111111116E-2</v>
-      </c>
-      <c r="E33" s="14" t="s">
+      <c r="D38" s="24">
+        <v>0.62361111111111112</v>
+      </c>
+      <c r="E38" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="H33" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="I33" s="14" t="s">
+      <c r="F38" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="I38" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="K33" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="L33" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="M33" s="27" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="3:13" ht="18" customHeight="1">
-      <c r="C34" s="17">
+      <c r="J38" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="L38" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="M38" s="26" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13" ht="18" customHeight="1">
+      <c r="C39" s="23">
         <v>43142</v>
       </c>
-      <c r="D34" s="15">
-        <v>0.37986111111111115</v>
-      </c>
-      <c r="E34" s="14" t="s">
+      <c r="D39" s="24">
+        <v>0.65833333333333333</v>
+      </c>
+      <c r="E39" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="H34" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="I34" s="14" t="s">
+      <c r="F39" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="H39" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="I39" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J34" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="K34" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="L34" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="M34" s="27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="3:13" ht="18" customHeight="1">
-      <c r="C35" s="17">
+      <c r="J39" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="K39" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="L39" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="M39" s="26" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13" ht="18" customHeight="1">
+      <c r="C40" s="23">
         <v>43142</v>
       </c>
-      <c r="D35" s="15">
-        <v>0.46319444444444446</v>
-      </c>
-      <c r="E35" s="14" t="s">
+      <c r="D40" s="24">
+        <v>0.81111111111111101</v>
+      </c>
+      <c r="E40" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="H35" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="I35" s="14" t="s">
+      <c r="F40" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="H40" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="I40" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="K35" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="L35" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="M35" s="27" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="3:13" ht="18" customHeight="1">
-      <c r="C36" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D36" s="15">
-        <v>0.56111111111111112</v>
-      </c>
-      <c r="E36" s="14" t="s">
+      <c r="J40" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="L40" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="M40" s="26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="41" spans="3:13" ht="18" customHeight="1">
+      <c r="C41" s="23">
+        <v>43143</v>
+      </c>
+      <c r="D41" s="24">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="E41" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="H36" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="I36" s="14" t="s">
+      <c r="F41" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="I41" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J36" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="K36" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="L36" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="M36" s="27" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="37" spans="3:13" ht="18" customHeight="1">
-      <c r="C37" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D37" s="15">
-        <v>0.57152777777777775</v>
-      </c>
-      <c r="E37" s="14" t="s">
+      <c r="J41" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="K41" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="L41" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="M41" s="26" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="3:13" ht="18" customHeight="1">
+      <c r="C42" s="23">
+        <v>43143</v>
+      </c>
+      <c r="D42" s="15">
+        <v>8.4722222222222213E-2</v>
+      </c>
+      <c r="E42" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F37" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="H37" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J37" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="K37" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="L37" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="M37" s="27" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="38" spans="3:13" ht="18" customHeight="1">
-      <c r="C38" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D38" s="15">
-        <v>0.62361111111111112</v>
-      </c>
-      <c r="E38" s="14" t="s">
+      <c r="F42" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="H42" s="21"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="22"/>
+    </row>
+    <row r="43" spans="3:13" ht="18" customHeight="1">
+      <c r="C43" s="17"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="H38" s="32" t="s">
-        <v>187</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J38" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="K38" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="L38" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="M38" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="3:13" ht="18" customHeight="1">
-      <c r="C39" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D39" s="15">
-        <v>0.65833333333333333</v>
-      </c>
-      <c r="E39" s="14" t="s">
+      <c r="F43" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="K43" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="L43" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="M43" s="22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13" ht="18" customHeight="1">
+      <c r="C44" s="17"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="H39" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J39" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="K39" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="L39" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="M39" s="27" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="40" spans="3:13" ht="18" customHeight="1">
-      <c r="C40" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D40" s="15">
-        <v>0.81111111111111101</v>
-      </c>
-      <c r="E40" s="14" t="s">
+      <c r="I44" s="14"/>
+    </row>
+    <row r="45" spans="3:13" ht="18" customHeight="1">
+      <c r="C45" s="17"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="H40" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="I40" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J40" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="K40" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="L40" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="M40" s="27" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="41" spans="3:13" ht="18" customHeight="1">
-      <c r="C41" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D41" s="15">
-        <v>0.56111111111111112</v>
-      </c>
-      <c r="E41" s="14" t="s">
+      <c r="I45" s="14"/>
+    </row>
+    <row r="46" spans="3:13" ht="18" customHeight="1">
+      <c r="C46" s="17"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="H41" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="J41" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="3:13" ht="18" customHeight="1">
-      <c r="C42" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D42" s="15">
-        <v>2.2916666666666669E-2</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="3:13" ht="18" customHeight="1">
-      <c r="C43" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D43" s="15">
-        <v>2.2916666666666669E-2</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="3:13" ht="18" customHeight="1">
-      <c r="C44" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D44" s="15">
-        <v>2.2916666666666669E-2</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="3:13" ht="18" customHeight="1">
-      <c r="C45" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D45" s="15">
-        <v>2.2916666666666669E-2</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="3:13" ht="18" customHeight="1">
-      <c r="C46" s="17">
-        <v>43142</v>
-      </c>
-      <c r="D46" s="15">
-        <v>2.2916666666666669E-2</v>
-      </c>
+      <c r="I46" s="14"/>
     </row>
     <row r="47" spans="3:13" ht="18" customHeight="1">
       <c r="C47" s="17"/>
-      <c r="D47" s="15">
-        <v>2.2916666666666669E-2</v>
-      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="14"/>
     </row>
     <row r="48" spans="3:13" ht="18" customHeight="1">
       <c r="C48" s="17"/>
       <c r="D48" s="15"/>
+      <c r="I48" s="14"/>
     </row>
     <row r="49" spans="3:4" ht="18" customHeight="1">
       <c r="C49" s="17"/>
@@ -6017,19 +5513,19 @@
       <c r="C327" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E14:E55 C13:D55 G37:G55 F42:F55 H42:H55 I41:I55 K41:K55 J42:J55">
-    <cfRule type="expression" dxfId="17" priority="4">
+  <conditionalFormatting sqref="J44:K55 I49:I55 G37:G40 C13:D55 E14:E55 F44:H55">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>#REF!="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="G37:G55 F42:F55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This course  isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Course List sheet, it will automatically appear in the list." sqref="G37:G40 F44:G55">
       <formula1>Courses</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This employee name isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Personnel Info sheet, it will automatically appear in the list." sqref="E46:E55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="Whoops!" error="This employee name isn’t in the drop down list. If what you typed isn’t a mistake you can click Yes and use it anyway. If you add the name the Personnel Info sheet, it will automatically appear in the list." sqref="E48:E55">
       <formula1>Employees</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="H42:H55 I41:I55 J42:J55">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Whoops!" error="This should be a Yes or No value." sqref="I49:I55 J44:J55 H44:H55">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6064,102 +5560,106 @@
     <hyperlink ref="E39" r:id="rId28" display="https://github.com/Spirovanni/Blackshields/commits?author=Spirovanni"/>
     <hyperlink ref="E40" r:id="rId29" display="https://github.com/Spirovanni/Blackshields/commits?author=Spirovanni"/>
     <hyperlink ref="E41" r:id="rId30" display="https://github.com/Spirovanni/Blackshields/commits?author=Spirovanni"/>
-    <hyperlink ref="E42" r:id="rId31" display="https://github.com/Spirovanni/Blackshields/commits?author=Spirovanni"/>
-    <hyperlink ref="E43" r:id="rId32" display="https://github.com/Spirovanni/Blackshields/commits?author=Spirovanni"/>
-    <hyperlink ref="E44" r:id="rId33" display="https://github.com/Spirovanni/Blackshields/commits?author=Spirovanni"/>
-    <hyperlink ref="E45" r:id="rId34" display="https://github.com/Spirovanni/Blackshields/commits?author=Spirovanni"/>
-    <hyperlink ref="K14" r:id="rId35" display="https://github.com/Spirovanni/Pirate-Castle/commit/5f2199f4cf52f8fa4d90707a6073c41afae61bcf"/>
-    <hyperlink ref="J14" r:id="rId36" tooltip="Merged Pull Request: 0. Version added to README.md" display="https://github.com/Spirovanni/Pirate-Castle/pull/1"/>
-    <hyperlink ref="I14" r:id="rId37" display="https://github.com/Spirovanni/Pirate-Castle"/>
-    <hyperlink ref="J15" r:id="rId38" tooltip="Merged Pull Request: 1.  Added &quot;barbican&quot; and &quot;registry&quot; directory" display="https://github.com/Spirovanni/Pirate-Castle/pull/2"/>
-    <hyperlink ref="I15:I40" r:id="rId39" display="https://github.com/Spirovanni/Pirate-Castle"/>
-    <hyperlink ref="K15" r:id="rId40" display="https://github.com/Spirovanni/Pirate-Castle/commit/56d2d5e17e4c7ef5b9408e639fad07ddb648a8f2"/>
-    <hyperlink ref="K16" r:id="rId41" display="https://github.com/Spirovanni/Pirate-Castle/commit/9ba6b022fbe34293ee459f682bf32e0ddde23494"/>
-    <hyperlink ref="J16" r:id="rId42" tooltip="Merged Pull Request: 2. Generated jhipster in &quot;barbican&quot; folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/3"/>
-    <hyperlink ref="F17" r:id="rId43" tooltip="3. Added &quot;registry&quot; files from github_x000a__x000a_Add &quot;version&quot;: &quot;3.2.4&quot;, to registry folder" display="https://github.com/Spirovanni/Pirate-Castle/commit/157613ac95fb783a249dd083f17e13a22ce90a40"/>
-    <hyperlink ref="J17" r:id="rId44" tooltip="Merged Pull Request: 3. Added &quot;registry&quot; files from github" display="https://github.com/Spirovanni/Pirate-Castle/pull/4"/>
-    <hyperlink ref="K17" r:id="rId45" display="https://github.com/Spirovanni/Pirate-Castle/commit/5a16089bca5dbf91aff00987f2817cf484984adb"/>
-    <hyperlink ref="F16" r:id="rId46" tooltip="2. Generated jhipster in &quot;barbican&quot; folder_x000a__x000a_Application files will be generated in folder: C:\Users\Staff2\dev\Pirate-Castle\barbican_x000a_? Which *type* of application would you like to create? Microservice gateway_x000a_? What is the base name of your application?" display="https://github.com/Spirovanni/Pirate-Castle/commit/5a16089bca5dbf91aff00987f2817cf484984adb"/>
-    <hyperlink ref="F15" r:id="rId47" tooltip="1.  Added &quot;barbican&quot; and &quot;registry&quot; directory_x000a__x000a_C:\Users\Staff2\dev\Pirate-Castle&gt;mkdir registry &amp; mkdir barbican" display="https://github.com/Spirovanni/Pirate-Castle/commit/9ba6b022fbe34293ee459f682bf32e0ddde23494"/>
-    <hyperlink ref="F14" r:id="rId48" tooltip="0. Version added to README.md_x000a__x000a_First update from GitKraken" display="https://github.com/Spirovanni/Pirate-Castle/commit/56d2d5e17e4c7ef5b9408e639fad07ddb648a8f2"/>
-    <hyperlink ref="F18" r:id="rId49" tooltip="4. Dependency merge;_x000a__x000a_We need to add dependencies to package.json from ngx-admin/package.json that is not exists. Also you need to check version of dependency that is already exists. You can pick ngx-admin version if it is upper." display="https://github.com/Spirovanni/Pirate-Castle/commit/f808899cd659b6f1b7d643304a93c850ef924724"/>
-    <hyperlink ref="J18" r:id="rId50" tooltip="Merged Pull Request: 4. Dependency merge;" display="https://github.com/Spirovanni/Pirate-Castle/pull/5"/>
-    <hyperlink ref="K18" r:id="rId51" display="https://github.com/Spirovanni/Pirate-Castle/commit/157613ac95fb783a249dd083f17e13a22ce90a40"/>
-    <hyperlink ref="F19" r:id="rId52" tooltip="5. Copy ngx-admin ui-component files;_x000a__x000a_mkdir src/main/webapp/app/ngx-admin;_x000a_cp -R ../ngx-admin/src/app/* src/main/webapp/app/ngx-admin/" display="https://github.com/Spirovanni/Pirate-Castle/commit/f3d4bd83b06bd8d5cd95ce38960b6a82fb221a5c"/>
-    <hyperlink ref="J19" r:id="rId53" tooltip="Merged Pull Request: 5. Copy ngx-admin ui-component files;" display="https://github.com/Spirovanni/Pirate-Castle/pull/6"/>
-    <hyperlink ref="K19" r:id="rId54" display="https://github.com/Spirovanni/Pirate-Castle/commit/f808899cd659b6f1b7d643304a93c850ef924724"/>
-    <hyperlink ref="F20" r:id="rId55" tooltip="6. bootstrapModule switched to ngx-admin app-module_x000a__x000a_Updated &quot;app.main.ts&quot; file." display="https://github.com/Spirovanni/Pirate-Castle/commit/39858907d928bca6401f2c6e8a0af5a5ec8e9b66"/>
-    <hyperlink ref="J20" r:id="rId56" tooltip="Merged Pull Request: 6. bootstrapModule switched to ngx-admin app-module" display="https://github.com/Spirovanni/Pirate-Castle/pull/7"/>
-    <hyperlink ref="K20" r:id="rId57" display="https://github.com/Spirovanni/Pirate-Castle/commit/f3d4bd83b06bd8d5cd95ce38960b6a82fb221a5c"/>
-    <hyperlink ref="F21" r:id="rId58" tooltip="7. Overwrite index.html from ngx-admin_x000a__x000a_cp ../ngx-admin/src/index.html src/main/webapp/index.html" display="https://github.com/Spirovanni/Pirate-Castle/commit/69dadbfad32c827cecb95c9b367c3de783686e0a"/>
-    <hyperlink ref="J21" r:id="rId59" tooltip="Merged Pull Request: 7. Overwrite index.html from ngx-admin" display="https://github.com/Spirovanni/Pirate-Castle/pull/8"/>
-    <hyperlink ref="K21" r:id="rId60" display="https://github.com/Spirovanni/Pirate-Castle/commit/39858907d928bca6401f2c6e8a0af5a5ec8e9b66"/>
-    <hyperlink ref="F22" r:id="rId61" tooltip="9. Fix &quot;Cannot find name 'tinymce'&quot; error_x000a__x000a_cp ../ngx-admin/src/typings.d.ts src/main/webapp/app/ngx-admin/_x000a_and import it in app-module" display="https://github.com/Spirovanni/Pirate-Castle/commit/5d289bfe0f7312af450d76f10b941b4ebd23f8b9"/>
-    <hyperlink ref="J22" r:id="rId62" tooltip="Merged Pull Request: 9. Fix &quot;Cannot find name 'tinymce'&quot; error" display="https://github.com/Spirovanni/Pirate-Castle/pull/9"/>
-    <hyperlink ref="K22" r:id="rId63" display="https://github.com/Spirovanni/Pirate-Castle/commit/69dadbfad32c827cecb95c9b367c3de783686e0a"/>
-    <hyperlink ref="F23" r:id="rId64" tooltip="10. Fix Error: Cannot find module 'app/pages/pages.module'._x000a__x000a_Setting a clean path" display="https://github.com/Spirovanni/Pirate-Castle/commit/2e901a51134984e3cf4a46e4f000f9bf629b9d28"/>
-    <hyperlink ref="J23" r:id="rId65" tooltip="Merged Pull Request: 10. Fix Error: Cannot find module 'app/pages/pages.module'." display="https://github.com/Spirovanni/Pirate-Castle/pull/10"/>
-    <hyperlink ref="K23" r:id="rId66" display="https://github.com/Spirovanni/Pirate-Castle/commit/5d289bfe0f7312af450d76f10b941b4ebd23f8b9"/>
-    <hyperlink ref="F24" r:id="rId67" tooltip="11. Copy the assets folder_x000a__x000a_cp -R ../ngx-admin/src/assets ./src/main/webapp/app/ngx-admin/" display="https://github.com/Spirovanni/Pirate-Castle/commit/0e436298741ae99a17beacbdfc7ce587d7f03fda"/>
-    <hyperlink ref="J24" r:id="rId68" tooltip="Merged Pull Request: 11. Copy the assets folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/11"/>
-    <hyperlink ref="K24" r:id="rId69" display="https://github.com/Spirovanni/Pirate-Castle/commit/2e901a51134984e3cf4a46e4f000f9bf629b9d28"/>
-    <hyperlink ref="F25" r:id="rId70" tooltip="12. Configure webpack/webpack.common.js to copy assets folder to targt we…_x000a__x000a_…b folder to be able to served from application" display="https://github.com/Spirovanni/Pirate-Castle/commit/ef60494acc6a007fa853cd1557175e4ce52e4b30"/>
-    <hyperlink ref="J25" r:id="rId71" tooltip="Merged Pull Request: 12. Configure webpack/webpack.common.js to copy assets folder to targ…" display="https://github.com/Spirovanni/Pirate-Castle/pull/12"/>
-    <hyperlink ref="K25" r:id="rId72" display="https://github.com/Spirovanni/Pirate-Castle/commit/0e436298741ae99a17beacbdfc7ce587d7f03fda"/>
-    <hyperlink ref="F26" r:id="rId73" tooltip="13. Location update for new assets folder in rooms component scss_x000a__x000a_Location change because of positioning" display="https://github.com/Spirovanni/Pirate-Castle/commit/d8f32fab62468081b5d66cf40e12068572e4c21f"/>
-    <hyperlink ref="J26" r:id="rId74" tooltip="Merged Pull Request: 13. Location update for new assets folder in rooms component scss" display="https://github.com/Spirovanni/Pirate-Castle/pull/13"/>
-    <hyperlink ref="K26" r:id="rId75" display="https://github.com/Spirovanni/Pirate-Castle/commit/ef60494acc6a007fa853cd1557175e4ce52e4b30"/>
-    <hyperlink ref="F27" r:id="rId76" tooltip="14. Import ngx-admin theme and styles config in vendor.scss_x000a__x000a_Connecting SCSS files" display="https://github.com/Spirovanni/Pirate-Castle/commit/b82c1fd4f4ea02cceb9f786aac12ea88ac0eb1c9"/>
-    <hyperlink ref="J27" r:id="rId77" tooltip="Merged Pull Request: 14. Import ngx-admin theme and styles config in vendor.scss" display="https://github.com/Spirovanni/Pirate-Castle/pull/14"/>
-    <hyperlink ref="K27" r:id="rId78" display="https://github.com/Spirovanni/Pirate-Castle/commit/d8f32fab62468081b5d66cf40e12068572e4c21f"/>
-    <hyperlink ref="F28" r:id="rId79" tooltip="15. Clear jhipster bootstrap style configs that can conflict with_x000a__x000a_ngx-admin styles" display="https://github.com/Spirovanni/Pirate-Castle/commit/327e5ddc66f329c757c423fef55590b75726dfeb"/>
-    <hyperlink ref="J28" r:id="rId80" tooltip="Merged Pull Request: 15. Clear jhipster bootstrap style configs that can conflict with" display="https://github.com/Spirovanni/Pirate-Castle/pull/15"/>
-    <hyperlink ref="K28" r:id="rId81" display="https://github.com/Spirovanni/Pirate-Castle/commit/b82c1fd4f4ea02cceb9f786aac12ea88ac0eb1c9"/>
-    <hyperlink ref="F29" r:id="rId82" tooltip="17. Echarts dependency install and compnent configs applied._x000a__x000a_npm install echarts@3.7.2 --save;" display="https://github.com/Spirovanni/Pirate-Castle/commit/d481422865fb0045eecc23700b50649ffd1be0db"/>
-    <hyperlink ref="J29" r:id="rId83" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/16"/>
-    <hyperlink ref="K29" r:id="rId84" display="https://github.com/Spirovanni/Pirate-Castle/commit/70338c0506ae76b4d289c0bee4a0b3d96344f399"/>
-    <hyperlink ref="F30" r:id="rId85" tooltip="18. tinymce and chart components js bundle configs" display="https://github.com/Spirovanni/Pirate-Castle/commit/fb44622459762e704b049cc0f3d672a01d5e69a8"/>
-    <hyperlink ref="J30" r:id="rId86" tooltip="Merged Pull Request: 18. tinymce and chart components js bundle configs" display="https://github.com/Spirovanni/Pirate-Castle/pull/17"/>
-    <hyperlink ref="K30" r:id="rId87" display="https://github.com/Spirovanni/Pirate-Castle/commit/d481422865fb0045eecc23700b50649ffd1be0db"/>
-    <hyperlink ref="F31" r:id="rId88" tooltip="18. String based lazy router loading fixes." display="https://github.com/Spirovanni/Pirate-Castle/commit/6cef9c251affc1695a2b4bda5a3fa66ac419a283"/>
-    <hyperlink ref="J31" r:id="rId89" tooltip="Merged Pull Request: 18. String based lazy router loading fixes." display="https://github.com/Spirovanni/Pirate-Castle/pull/18"/>
-    <hyperlink ref="K31" r:id="rId90" display="https://github.com/Spirovanni/Pirate-Castle/commit/fb44622459762e704b049cc0f3d672a01d5e69a8"/>
-    <hyperlink ref="F32" r:id="rId91" tooltip="19. Echarts world component js added_x000a__x000a_None" display="https://github.com/Spirovanni/Pirate-Castle/commit/3628054f0bfea6114f7867d8febf92d3ca38ca0f"/>
-    <hyperlink ref="J32" r:id="rId92" tooltip="Merged Pull Request: 19. Echarts world component js added" display="https://github.com/Spirovanni/Pirate-Castle/pull/19"/>
-    <hyperlink ref="K32" r:id="rId93" display="https://github.com/Spirovanni/Pirate-Castle/commit/6cef9c251affc1695a2b4bda5a3fa66ac419a283"/>
-    <hyperlink ref="F33" r:id="rId94" tooltip="20. Adding Doc folder_x000a__x000a_created scripts.txt file" display="https://github.com/Spirovanni/Pirate-Castle/commit/4187afd07e808429beb3e235e4bc8bff6758e488"/>
-    <hyperlink ref="J33" r:id="rId95" tooltip="Merged Pull Request: 20. Adding Doc folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/20"/>
-    <hyperlink ref="K33" r:id="rId96" display="https://github.com/Spirovanni/Pirate-Castle/commit/3628054f0bfea6114f7867d8febf92d3ca38ca0f"/>
-    <hyperlink ref="F34" r:id="rId97" tooltip="21. Updated charts folder_x000a__x000a_Replaced &quot;ngx&quot; with &quot;jhi&quot; in selectors." display="https://github.com/Spirovanni/Pirate-Castle/commit/06e453d6b28e0969123cc65cccd5220f7a7bfab0"/>
-    <hyperlink ref="J34" r:id="rId98" tooltip="Merged Pull Request: 21. Updated charts folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/21"/>
-    <hyperlink ref="K34" r:id="rId99" display="https://github.com/Spirovanni/Pirate-Castle/commit/4187afd07e808429beb3e235e4bc8bff6758e488"/>
-    <hyperlink ref="F35" r:id="rId100" tooltip="22. Update &quot;@theme/ components &amp; layouts&quot;_x000a__x000a_Replaced &quot;ngx&quot; with &quot;jhi&quot; in selectors." display="https://github.com/Spirovanni/Pirate-Castle/commit/9893d85e59b5ee28753c1ae2080bf9cc42011a2e"/>
-    <hyperlink ref="J35" r:id="rId101" tooltip="Merged Pull Request: 22. Update &quot;@theme/ components &amp; layouts&quot;" display="https://github.com/Spirovanni/Pirate-Castle/pull/22"/>
-    <hyperlink ref="K35" r:id="rId102" display="https://github.com/Spirovanni/Pirate-Castle/commit/06e453d6b28e0969123cc65cccd5220f7a7bfab0"/>
-    <hyperlink ref="F36" r:id="rId103" tooltip="23. Updated the other files in &quot;@theme/ components &amp; layouts&quot;_x000a__x000a_Replaced &quot;ngx&quot; with &quot;jhi&quot; in selectors." display="https://github.com/Spirovanni/Pirate-Castle/commit/0df7406dc2e38e3a4b036b4aabad0d4be6078453"/>
-    <hyperlink ref="J36" r:id="rId104" tooltip="Merged Pull Request: 23. Updated the other files in &quot;@theme/ components &amp; layouts&quot;" display="https://github.com/Spirovanni/Pirate-Castle/pull/23"/>
-    <hyperlink ref="F37" r:id="rId105" tooltip="24. Corrected Warnings in pages/charts folder_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-multiple-xaxis.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-pie.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-radar.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-line.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-bar.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-bar-horizontal.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition" display="https://github.com/Spirovanni/Pirate-Castle/commit/9b2460bfab1deef0ad4a2262cca728baee354eb9"/>
-    <hyperlink ref="J37" r:id="rId106" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/24"/>
-    <hyperlink ref="K37" r:id="rId107" display="https://github.com/Spirovanni/Pirate-Castle/commit/0df7406dc2e38e3a4b036b4aabad0d4be6078453"/>
-    <hyperlink ref="K36" r:id="rId108" display="https://github.com/Spirovanni/Pirate-Castle/commit/9893d85e59b5ee28753c1ae2080bf9cc42011a2e"/>
-    <hyperlink ref="F38" r:id="rId109" tooltip="25. Corrected Warnings in pages/charts/echarts folder_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/ui-features/buttons/hero-buttons/hero-buttons.component.ts_x000a_[16, 71]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-area-stack.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsAreaStackComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-bar.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsBarComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-line.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsLineComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-pie.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsPieComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-radar.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsRadarComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-multiple-xaxis.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_[61, 28]: Parentheses are required around the parameters of an arrow function definition_x000a_[101, 28]: Parentheses are required around the parameters of an arrow function definition_x000a_[5, 13]: The selector of the component &quot;EchartsMultipleXaxisComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts-bar-animation.component.ts_x000a_[18, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_ [5, 13]: The selector of the component &quot;EchartsBarAnimationComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)" display="https://github.com/Spirovanni/Pirate-Castle/commit/f141dd65d9d4cae1e8b0eea04951a6291cf83e15"/>
-    <hyperlink ref="J38" r:id="rId110" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/24"/>
-    <hyperlink ref="K38" r:id="rId111" display="https://github.com/Spirovanni/Pirate-Castle/commit/9b2460bfab1deef0ad4a2262cca728baee354eb9"/>
-    <hyperlink ref="F39" r:id="rId112" tooltip="25b. Corrected Warnings in @theme/components/tiny-mce files_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/@theme/components/tiny-mce/tiny-mce.component.ts_x000a_[20, 14]: Parentheses are required around the parameters of an arrow function definition" display="https://github.com/Spirovanni/Pirate-Castle/commit/46fd768d0688f5522aec5c767af3f2fb840d10fa"/>
-    <hyperlink ref="K39" r:id="rId113" display="https://github.com/Spirovanni/Pirate-Castle/commit/f141dd65d9d4cae1e8b0eea04951a6291cf83e15"/>
-    <hyperlink ref="J39" r:id="rId114" tooltip="Merged Pull Request: 25b. Corrected Warnings in @theme/components/tiny-mce files" display="https://github.com/Spirovanni/Pirate-Castle/pull/25"/>
-    <hyperlink ref="F40" r:id="rId115" tooltip="26. Corrected Warning in various files_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/dashboard.module.ts_x000a_[23, 1]: Consecutive blank lines are forbidden_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/temperature/temperature.component.ts_x000a_[23, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/electricity/electricity.component.ts_x000a_[24, 71]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/traffic/traffic-chart.component.ts_x000a_[26, 73]: Parentheses are required around the parameters of an arrow function definition_x000a_[101, 30]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/d3/d3-pie.component.ts_x000a_[27, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/maps/bubble/bubble-map.component.ts_x000a_[31, 18]: Parentheses are required around the parameters of an arrow function definition_x000a_[471, 24]: Parentheses are required around the parameters of an arrow function definition_x000a_[508, 38]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/d3/d3-advanced-pie.component.ts_x000a_[32, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/traffic/traffic.component.ts_x000a_[34, 71]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/echarts/echarts.component.ts_x000a_[4, 13]: The selector of the component &quot;EchartsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/editors/editors.component.ts_x000a_[4, 13]: The selector of the component &quot;EditorsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/forms/form-inputs/form-inputs.component.ts_x000a_[4, 13]: The selector of the component &quot;FormInputsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/forms/form-layouts/form-layouts.component.ts_x000a_[4, 13]: The selector of the component &quot;FormLayoutsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/forms/forms.component.ts_x000a_[4, 13]: The selector of the component &quot;FormsComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/editors/tiny-mce/tiny-mce.component.ts_x000a_[4, 13]: The selector of the component &quot;TinyMCEComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/@core/core.module.ts_x000a_[41, 3]: Declaration of static method not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/solar/solar.component.ts_x000a_[44, 73]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/electricity/electricity-chart/electricity-chart.component.ts_x000a_[44, 73]: Parentheses are required around the parameters of an arrow function definition_x000a_[79, 33]: Parentheses are required around the parameters of an arrow function definition_x000a_[158, 35]: Parentheses are required around the parameters of an arrow function definition_x000a_[181, 35]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/components/tree/tree.component.ts_x000a_[5, 13]: The selector of the component &quot;TreeComponent&quot; should have prefix &quot;jhi&quot; (https://angular.io/styleguide#style-02-07)_x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/temperature/temperature-dragger/temperature-dragger.component.ts_x000a_[52, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[53, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[55, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[56, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[57, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[58, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[59, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[60, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[61, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[62, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[63, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[65, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[75, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[76, 3]: Declaration of instance field not allowed after declaration of instance method. Instead, this should come at the beginning of the class/interface._x000a_[350, 3]: Declaration of static method not allowed after declaration of instance method. Instead, this should come after instance fields._x000a_[143, 1]: Consecutive blank lines are forbidden" display="https://github.com/Spirovanni/Pirate-Castle/commit/06e78f523f84a35f073a7b9e7615208f9b8c07c7"/>
-    <hyperlink ref="J40" r:id="rId116" tooltip="Merged Pull Request: 26. Corrected Warning in various files" display="https://github.com/Spirovanni/Pirate-Castle/pull/26"/>
-    <hyperlink ref="K40" r:id="rId117" display="https://github.com/Spirovanni/Pirate-Castle/commit/46fd768d0688f5522aec5c767af3f2fb840d10fa"/>
-    <hyperlink ref="F41" r:id="rId118" tooltip="27. Fixed last warnings_x000a__x000a_Ran without warnings" display="https://github.com/Spirovanni/Pirate-Castle/commit/535df5af0e73b859e37a4f1accd7af8008d3a3ce"/>
-    <hyperlink ref="J41" r:id="rId119" tooltip="Merged Pull Request: 27. Fixed last warnings" display="https://github.com/Spirovanni/Pirate-Castle/pull/27"/>
+    <hyperlink ref="K14" r:id="rId31" display="https://github.com/Spirovanni/Pirate-Castle/commit/5f2199f4cf52f8fa4d90707a6073c41afae61bcf"/>
+    <hyperlink ref="J14" r:id="rId32" tooltip="Merged Pull Request: 0. Version added to README.md" display="https://github.com/Spirovanni/Pirate-Castle/pull/1"/>
+    <hyperlink ref="I14" r:id="rId33" display="https://github.com/Spirovanni/Pirate-Castle"/>
+    <hyperlink ref="J15" r:id="rId34" tooltip="Merged Pull Request: 1.  Added &quot;barbican&quot; and &quot;registry&quot; directory" display="https://github.com/Spirovanni/Pirate-Castle/pull/2"/>
+    <hyperlink ref="I15:I40" r:id="rId35" display="https://github.com/Spirovanni/Pirate-Castle"/>
+    <hyperlink ref="K15" r:id="rId36" display="https://github.com/Spirovanni/Pirate-Castle/commit/56d2d5e17e4c7ef5b9408e639fad07ddb648a8f2"/>
+    <hyperlink ref="K16" r:id="rId37" display="https://github.com/Spirovanni/Pirate-Castle/commit/9ba6b022fbe34293ee459f682bf32e0ddde23494"/>
+    <hyperlink ref="J16" r:id="rId38" tooltip="Merged Pull Request: 2. Generated jhipster in &quot;barbican&quot; folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/3"/>
+    <hyperlink ref="F17" r:id="rId39" tooltip="3. Added &quot;registry&quot; files from github_x000a__x000a_Add &quot;version&quot;: &quot;3.2.4&quot;, to registry folder" display="https://github.com/Spirovanni/Pirate-Castle/commit/157613ac95fb783a249dd083f17e13a22ce90a40"/>
+    <hyperlink ref="J17" r:id="rId40" tooltip="Merged Pull Request: 3. Added &quot;registry&quot; files from github" display="https://github.com/Spirovanni/Pirate-Castle/pull/4"/>
+    <hyperlink ref="K17" r:id="rId41" display="https://github.com/Spirovanni/Pirate-Castle/commit/5a16089bca5dbf91aff00987f2817cf484984adb"/>
+    <hyperlink ref="F16" r:id="rId42" tooltip="2. Generated jhipster in &quot;barbican&quot; folder_x000a__x000a_Application files will be generated in folder: C:\Users\Staff2\dev\Pirate-Castle\barbican_x000a_? Which *type* of application would you like to create? Microservice gateway_x000a_? What is the base name of your application?" display="https://github.com/Spirovanni/Pirate-Castle/commit/5a16089bca5dbf91aff00987f2817cf484984adb"/>
+    <hyperlink ref="F15" r:id="rId43" tooltip="1.  Added &quot;barbican&quot; and &quot;registry&quot; directory_x000a__x000a_C:\Users\Staff2\dev\Pirate-Castle&gt;mkdir registry &amp; mkdir barbican" display="https://github.com/Spirovanni/Pirate-Castle/commit/9ba6b022fbe34293ee459f682bf32e0ddde23494"/>
+    <hyperlink ref="F14" r:id="rId44" tooltip="0. Version added to README.md_x000a__x000a_First update from GitKraken" display="https://github.com/Spirovanni/Pirate-Castle/commit/56d2d5e17e4c7ef5b9408e639fad07ddb648a8f2"/>
+    <hyperlink ref="F18" r:id="rId45" tooltip="4. Dependency merge;_x000a__x000a_We need to add dependencies to package.json from ngx-admin/package.json that is not exists. Also you need to check version of dependency that is already exists. You can pick ngx-admin version if it is upper." display="https://github.com/Spirovanni/Pirate-Castle/commit/f808899cd659b6f1b7d643304a93c850ef924724"/>
+    <hyperlink ref="J18" r:id="rId46" tooltip="Merged Pull Request: 4. Dependency merge;" display="https://github.com/Spirovanni/Pirate-Castle/pull/5"/>
+    <hyperlink ref="K18" r:id="rId47" display="https://github.com/Spirovanni/Pirate-Castle/commit/157613ac95fb783a249dd083f17e13a22ce90a40"/>
+    <hyperlink ref="F19" r:id="rId48" tooltip="5. Copy ngx-admin ui-component files;_x000a__x000a_mkdir src/main/webapp/app/ngx-admin;_x000a_cp -R ../ngx-admin/src/app/* src/main/webapp/app/ngx-admin/" display="https://github.com/Spirovanni/Pirate-Castle/commit/f3d4bd83b06bd8d5cd95ce38960b6a82fb221a5c"/>
+    <hyperlink ref="J19" r:id="rId49" tooltip="Merged Pull Request: 5. Copy ngx-admin ui-component files;" display="https://github.com/Spirovanni/Pirate-Castle/pull/6"/>
+    <hyperlink ref="K19" r:id="rId50" display="https://github.com/Spirovanni/Pirate-Castle/commit/f808899cd659b6f1b7d643304a93c850ef924724"/>
+    <hyperlink ref="F20" r:id="rId51" tooltip="6. bootstrapModule switched to ngx-admin app-module_x000a__x000a_Updated &quot;app.main.ts&quot; file." display="https://github.com/Spirovanni/Pirate-Castle/commit/39858907d928bca6401f2c6e8a0af5a5ec8e9b66"/>
+    <hyperlink ref="J20" r:id="rId52" tooltip="Merged Pull Request: 6. bootstrapModule switched to ngx-admin app-module" display="https://github.com/Spirovanni/Pirate-Castle/pull/7"/>
+    <hyperlink ref="K20" r:id="rId53" display="https://github.com/Spirovanni/Pirate-Castle/commit/f3d4bd83b06bd8d5cd95ce38960b6a82fb221a5c"/>
+    <hyperlink ref="F21" r:id="rId54" tooltip="7. Overwrite index.html from ngx-admin_x000a__x000a_cp ../ngx-admin/src/index.html src/main/webapp/index.html" display="https://github.com/Spirovanni/Pirate-Castle/commit/69dadbfad32c827cecb95c9b367c3de783686e0a"/>
+    <hyperlink ref="J21" r:id="rId55" tooltip="Merged Pull Request: 7. Overwrite index.html from ngx-admin" display="https://github.com/Spirovanni/Pirate-Castle/pull/8"/>
+    <hyperlink ref="K21" r:id="rId56" display="https://github.com/Spirovanni/Pirate-Castle/commit/39858907d928bca6401f2c6e8a0af5a5ec8e9b66"/>
+    <hyperlink ref="F22" r:id="rId57" tooltip="9. Fix &quot;Cannot find name 'tinymce'&quot; error_x000a__x000a_cp ../ngx-admin/src/typings.d.ts src/main/webapp/app/ngx-admin/_x000a_and import it in app-module" display="https://github.com/Spirovanni/Pirate-Castle/commit/5d289bfe0f7312af450d76f10b941b4ebd23f8b9"/>
+    <hyperlink ref="J22" r:id="rId58" tooltip="Merged Pull Request: 9. Fix &quot;Cannot find name 'tinymce'&quot; error" display="https://github.com/Spirovanni/Pirate-Castle/pull/9"/>
+    <hyperlink ref="K22" r:id="rId59" display="https://github.com/Spirovanni/Pirate-Castle/commit/69dadbfad32c827cecb95c9b367c3de783686e0a"/>
+    <hyperlink ref="F23" r:id="rId60" tooltip="10. Fix Error: Cannot find module 'app/pages/pages.module'._x000a__x000a_Setting a clean path" display="https://github.com/Spirovanni/Pirate-Castle/commit/2e901a51134984e3cf4a46e4f000f9bf629b9d28"/>
+    <hyperlink ref="J23" r:id="rId61" tooltip="Merged Pull Request: 10. Fix Error: Cannot find module 'app/pages/pages.module'." display="https://github.com/Spirovanni/Pirate-Castle/pull/10"/>
+    <hyperlink ref="K23" r:id="rId62" display="https://github.com/Spirovanni/Pirate-Castle/commit/5d289bfe0f7312af450d76f10b941b4ebd23f8b9"/>
+    <hyperlink ref="F24" r:id="rId63" tooltip="11. Copy the assets folder_x000a__x000a_cp -R ../ngx-admin/src/assets ./src/main/webapp/app/ngx-admin/" display="https://github.com/Spirovanni/Pirate-Castle/commit/0e436298741ae99a17beacbdfc7ce587d7f03fda"/>
+    <hyperlink ref="J24" r:id="rId64" tooltip="Merged Pull Request: 11. Copy the assets folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/11"/>
+    <hyperlink ref="K24" r:id="rId65" display="https://github.com/Spirovanni/Pirate-Castle/commit/2e901a51134984e3cf4a46e4f000f9bf629b9d28"/>
+    <hyperlink ref="F25" r:id="rId66" tooltip="12. Configure webpack/webpack.common.js to copy assets folder to targt we…_x000a__x000a_…b folder to be able to served from application" display="https://github.com/Spirovanni/Pirate-Castle/commit/ef60494acc6a007fa853cd1557175e4ce52e4b30"/>
+    <hyperlink ref="J25" r:id="rId67" tooltip="Merged Pull Request: 12. Configure webpack/webpack.common.js to copy assets folder to targ…" display="https://github.com/Spirovanni/Pirate-Castle/pull/12"/>
+    <hyperlink ref="K25" r:id="rId68" display="https://github.com/Spirovanni/Pirate-Castle/commit/0e436298741ae99a17beacbdfc7ce587d7f03fda"/>
+    <hyperlink ref="F26" r:id="rId69" tooltip="13. Location update for new assets folder in rooms component scss_x000a__x000a_Location change because of positioning" display="https://github.com/Spirovanni/Pirate-Castle/commit/d8f32fab62468081b5d66cf40e12068572e4c21f"/>
+    <hyperlink ref="J26" r:id="rId70" tooltip="Merged Pull Request: 13. Location update for new assets folder in rooms component scss" display="https://github.com/Spirovanni/Pirate-Castle/pull/13"/>
+    <hyperlink ref="K26" r:id="rId71" display="https://github.com/Spirovanni/Pirate-Castle/commit/ef60494acc6a007fa853cd1557175e4ce52e4b30"/>
+    <hyperlink ref="F27" r:id="rId72" tooltip="14. Import ngx-admin theme and styles config in vendor.scss_x000a__x000a_Connecting SCSS files" display="https://github.com/Spirovanni/Pirate-Castle/commit/b82c1fd4f4ea02cceb9f786aac12ea88ac0eb1c9"/>
+    <hyperlink ref="J27" r:id="rId73" tooltip="Merged Pull Request: 14. Import ngx-admin theme and styles config in vendor.scss" display="https://github.com/Spirovanni/Pirate-Castle/pull/14"/>
+    <hyperlink ref="K27" r:id="rId74" display="https://github.com/Spirovanni/Pirate-Castle/commit/d8f32fab62468081b5d66cf40e12068572e4c21f"/>
+    <hyperlink ref="F28" r:id="rId75" tooltip="15. Clear jhipster bootstrap style configs that can conflict with_x000a__x000a_ngx-admin styles" display="https://github.com/Spirovanni/Pirate-Castle/commit/327e5ddc66f329c757c423fef55590b75726dfeb"/>
+    <hyperlink ref="J28" r:id="rId76" tooltip="Merged Pull Request: 15. Clear jhipster bootstrap style configs that can conflict with" display="https://github.com/Spirovanni/Pirate-Castle/pull/15"/>
+    <hyperlink ref="K28" r:id="rId77" display="https://github.com/Spirovanni/Pirate-Castle/commit/b82c1fd4f4ea02cceb9f786aac12ea88ac0eb1c9"/>
+    <hyperlink ref="F29" r:id="rId78" tooltip="17. Echarts dependency install and compnent configs applied._x000a__x000a_npm install echarts@3.7.2 --save;" display="https://github.com/Spirovanni/Pirate-Castle/commit/d481422865fb0045eecc23700b50649ffd1be0db"/>
+    <hyperlink ref="J29" r:id="rId79" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/16"/>
+    <hyperlink ref="K29" r:id="rId80" display="https://github.com/Spirovanni/Pirate-Castle/commit/70338c0506ae76b4d289c0bee4a0b3d96344f399"/>
+    <hyperlink ref="F30" r:id="rId81" tooltip="18. tinymce and chart components js bundle configs" display="https://github.com/Spirovanni/Pirate-Castle/commit/fb44622459762e704b049cc0f3d672a01d5e69a8"/>
+    <hyperlink ref="J30" r:id="rId82" tooltip="Merged Pull Request: 18. tinymce and chart components js bundle configs" display="https://github.com/Spirovanni/Pirate-Castle/pull/17"/>
+    <hyperlink ref="K30" r:id="rId83" display="https://github.com/Spirovanni/Pirate-Castle/commit/d481422865fb0045eecc23700b50649ffd1be0db"/>
+    <hyperlink ref="F31" r:id="rId84" tooltip="18. String based lazy router loading fixes." display="https://github.com/Spirovanni/Pirate-Castle/commit/6cef9c251affc1695a2b4bda5a3fa66ac419a283"/>
+    <hyperlink ref="J31" r:id="rId85" tooltip="Merged Pull Request: 18. String based lazy router loading fixes." display="https://github.com/Spirovanni/Pirate-Castle/pull/18"/>
+    <hyperlink ref="K31" r:id="rId86" display="https://github.com/Spirovanni/Pirate-Castle/commit/fb44622459762e704b049cc0f3d672a01d5e69a8"/>
+    <hyperlink ref="F32" r:id="rId87" tooltip="19. Echarts world component js added_x000a__x000a_None" display="https://github.com/Spirovanni/Pirate-Castle/commit/3628054f0bfea6114f7867d8febf92d3ca38ca0f"/>
+    <hyperlink ref="J32" r:id="rId88" tooltip="Merged Pull Request: 19. Echarts world component js added" display="https://github.com/Spirovanni/Pirate-Castle/pull/19"/>
+    <hyperlink ref="K32" r:id="rId89" display="https://github.com/Spirovanni/Pirate-Castle/commit/6cef9c251affc1695a2b4bda5a3fa66ac419a283"/>
+    <hyperlink ref="F33" r:id="rId90" tooltip="20. Adding Doc folder_x000a__x000a_created scripts.txt file" display="https://github.com/Spirovanni/Pirate-Castle/commit/4187afd07e808429beb3e235e4bc8bff6758e488"/>
+    <hyperlink ref="J33" r:id="rId91" tooltip="Merged Pull Request: 20. Adding Doc folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/20"/>
+    <hyperlink ref="K33" r:id="rId92" display="https://github.com/Spirovanni/Pirate-Castle/commit/3628054f0bfea6114f7867d8febf92d3ca38ca0f"/>
+    <hyperlink ref="F34" r:id="rId93" tooltip="21. Updated charts folder_x000a__x000a_Replaced &quot;ngx&quot; with &quot;jhi&quot; in selectors." display="https://github.com/Spirovanni/Pirate-Castle/commit/06e453d6b28e0969123cc65cccd5220f7a7bfab0"/>
+    <hyperlink ref="J34" r:id="rId94" tooltip="Merged Pull Request: 21. Updated charts folder" display="https://github.com/Spirovanni/Pirate-Castle/pull/21"/>
+    <hyperlink ref="K34" r:id="rId95" display="https://github.com/Spirovanni/Pirate-Castle/commit/4187afd07e808429beb3e235e4bc8bff6758e488"/>
+    <hyperlink ref="F35" r:id="rId96" tooltip="22. Update &quot;@theme/ components &amp; layouts&quot;_x000a__x000a_Replaced &quot;ngx&quot; with &quot;jhi&quot; in selectors." display="https://github.com/Spirovanni/Pirate-Castle/commit/9893d85e59b5ee28753c1ae2080bf9cc42011a2e"/>
+    <hyperlink ref="J35" r:id="rId97" tooltip="Merged Pull Request: 22. Update &quot;@theme/ components &amp; layouts&quot;" display="https://github.com/Spirovanni/Pirate-Castle/pull/22"/>
+    <hyperlink ref="K35" r:id="rId98" display="https://github.com/Spirovanni/Pirate-Castle/commit/06e453d6b28e0969123cc65cccd5220f7a7bfab0"/>
+    <hyperlink ref="F36" r:id="rId99" tooltip="23. Updated the other files in &quot;@theme/ components &amp; layouts&quot;_x000a__x000a_Replaced &quot;ngx&quot; with &quot;jhi&quot; in selectors." display="https://github.com/Spirovanni/Pirate-Castle/commit/0df7406dc2e38e3a4b036b4aabad0d4be6078453"/>
+    <hyperlink ref="J36" r:id="rId100" tooltip="Merged Pull Request: 23. Updated the other files in &quot;@theme/ components &amp; layouts&quot;" display="https://github.com/Spirovanni/Pirate-Castle/pull/23"/>
+    <hyperlink ref="F37" r:id="rId101" tooltip="24. Corrected Warnings in pages/charts folder_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/charts/chartjs/chartjs-multiple-xaxis.component.ts_x000a_[16, 64]: Parentheses are required around the parameters of an arrow function definition_x000a_WARNING in ./src/ma" display="https://github.com/Spirovanni/Pirate-Castle/commit/9b2460bfab1deef0ad4a2262cca728baee354eb9"/>
+    <hyperlink ref="J37" r:id="rId102" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/24"/>
+    <hyperlink ref="K37" r:id="rId103" display="https://github.com/Spirovanni/Pirate-Castle/commit/0df7406dc2e38e3a4b036b4aabad0d4be6078453"/>
+    <hyperlink ref="K36" r:id="rId104" display="https://github.com/Spirovanni/Pirate-Castle/commit/9893d85e59b5ee28753c1ae2080bf9cc42011a2e"/>
+    <hyperlink ref="F38" r:id="rId105" tooltip="25. Corrected Warnings in pages/charts/echarts folder_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/ui-features/buttons/hero-buttons/hero-buttons.component.ts_x000a_[16, 71]: Parentheses are required around the parameters of an arrow function definition_x000a_WAR" display="https://github.com/Spirovanni/Pirate-Castle/commit/f141dd65d9d4cae1e8b0eea04951a6291cf83e15"/>
+    <hyperlink ref="J38" r:id="rId106" tooltip="Merged Pull Request: Sand box" display="https://github.com/Spirovanni/Pirate-Castle/pull/24"/>
+    <hyperlink ref="K38" r:id="rId107" display="https://github.com/Spirovanni/Pirate-Castle/commit/9b2460bfab1deef0ad4a2262cca728baee354eb9"/>
+    <hyperlink ref="F39" r:id="rId108" tooltip="25b. Corrected Warnings in @theme/components/tiny-mce files_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/@theme/components/tiny-mce/tiny-mce.component.ts_x000a_[20, 14]: Parentheses are required around the parameters of an arrow function definition" display="https://github.com/Spirovanni/Pirate-Castle/commit/46fd768d0688f5522aec5c767af3f2fb840d10fa"/>
+    <hyperlink ref="K39" r:id="rId109" display="https://github.com/Spirovanni/Pirate-Castle/commit/f141dd65d9d4cae1e8b0eea04951a6291cf83e15"/>
+    <hyperlink ref="J39" r:id="rId110" tooltip="Merged Pull Request: 25b. Corrected Warnings in @theme/components/tiny-mce files" display="https://github.com/Spirovanni/Pirate-Castle/pull/25"/>
+    <hyperlink ref="F40" r:id="rId111" tooltip="26. Corrected Warning in various files_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/dashboard.module.ts_x000a_[23, 1]: Consecutive blank lines are forbidden_x000a__x000a_WARNING in ./src/main/webapp/app/ngx-admin/pages/dashboard/temperature/temperature.compo" display="https://github.com/Spirovanni/Pirate-Castle/commit/06e78f523f84a35f073a7b9e7615208f9b8c07c7"/>
+    <hyperlink ref="J40" r:id="rId112" tooltip="Merged Pull Request: 26. Corrected Warning in various files" display="https://github.com/Spirovanni/Pirate-Castle/pull/26"/>
+    <hyperlink ref="K40" r:id="rId113" display="https://github.com/Spirovanni/Pirate-Castle/commit/46fd768d0688f5522aec5c767af3f2fb840d10fa"/>
+    <hyperlink ref="F41" r:id="rId114" tooltip="27. Fixed last warnings_x000a__x000a_Ran without warnings" display="https://github.com/Spirovanni/Pirate-Castle/commit/535df5af0e73b859e37a4f1accd7af8008d3a3ce"/>
+    <hyperlink ref="J41" r:id="rId115" tooltip="Merged Pull Request: 27. Fixed last warnings" display="https://github.com/Spirovanni/Pirate-Castle/pull/27"/>
+    <hyperlink ref="K41" r:id="rId116" display="https://github.com/Spirovanni/Pirate-Castle/commit/06e78f523f84a35f073a7b9e7615208f9b8c07c7"/>
+    <hyperlink ref="I41:I48" r:id="rId117" display="https://github.com/Spirovanni/Pirate-Castle"/>
+    <hyperlink ref="F43" r:id="rId118" tooltip="29. Switched to &quot;jhi-main&quot; in index.html_x000a__x000a_Attempting to use original infastructure." display="https://github.com/Spirovanni/Pirate-Castle/commit/c3d9fc338ad245a0fde711a23669ef6cef73129d"/>
+    <hyperlink ref="F42" r:id="rId119" tooltip="28. Fixed all broken migration issues_x000a__x000a_MissionSuccess!!" display="https://github.com/Spirovanni/Pirate-Castle/commit/2fec5c3b6ad38de88615f06272c21b982356d34d"/>
+    <hyperlink ref="E42:E47" r:id="rId120" display="https://github.com/Spirovanni/Blackshields/commits?author=Spirovanni"/>
+    <hyperlink ref="I43" r:id="rId121" display="https://github.com/Spirovanni/Pirate-Castle"/>
+    <hyperlink ref="J43" r:id="rId122" tooltip="Merged Pull Request: 29. Switched to &quot;jhi-main&quot; in index.html" display="https://github.com/Spirovanni/Pirate-Castle/pull/29"/>
+    <hyperlink ref="K43" r:id="rId123" display="https://github.com/Spirovanni/Pirate-Castle/commit/2fec5c3b6ad38de88615f06272c21b982356d34d"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId120"/>
-  <drawing r:id="rId121"/>
+  <pageSetup scale="92" fitToHeight="0" orientation="landscape" r:id="rId124"/>
+  <drawing r:id="rId125"/>
   <tableParts count="1">
-    <tablePart r:id="rId122"/>
+    <tablePart r:id="rId126"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6339,7 +5839,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:C30 F6:F30">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>COUNTIF($C:$C,$C6)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6716,7 +6216,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:G50">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>(COUNTIF($C:$C,$C6)&gt;1)*($C6&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>